<commit_message>
Terasort results and resources
</commit_message>
<xml_diff>
--- a/resources/tools/YARNCalcs.xlsx
+++ b/resources/tools/YARNCalcs.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomma/SEBC/resources/tools/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="440" windowWidth="28160" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -265,6 +273,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -592,9 +605,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
@@ -604,12 +619,12 @@
     <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
@@ -618,7 +633,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -631,15 +646,15 @@
       </c>
       <c r="F2" s="7">
         <f>MIN(C15,PRODUCT(B2,2))</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="6" t="s">
@@ -647,10 +662,10 @@
       </c>
       <c r="F3" s="7">
         <f>PRODUCT(B15,1024)</f>
-        <v>232857.60000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+        <v>114892.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -664,12 +679,12 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="6" t="s">
@@ -679,7 +694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D6" s="3"/>
       <c r="E6" s="6" t="s">
         <v>10</v>
@@ -688,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6"/>
       <c r="B7" s="9" t="s">
         <v>11</v>
@@ -704,13 +719,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="7">
         <f>PRODUCT(0.1,B3)</f>
-        <v>25.6</v>
+        <v>12.8</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -723,7 +738,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -739,10 +754,10 @@
       </c>
       <c r="F9" s="11">
         <f>PRODUCT(F2,1024)</f>
-        <v>24576</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+        <v>15360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
@@ -760,7 +775,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -779,7 +794,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
@@ -798,10 +813,10 @@
       </c>
       <c r="G12" s="7">
         <f>F3/F12</f>
-        <v>227.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+        <v>112.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
@@ -822,7 +837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
@@ -841,20 +856,20 @@
       </c>
       <c r="G14" s="7">
         <f>F2/F14</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="7">
         <f>SUM(B3,-B8,-B9,-B10,-B11,-B12,-B13,-B14)</f>
-        <v>227.4</v>
+        <v>112.2</v>
       </c>
       <c r="C15" s="7">
         <f>SUM(B1,-C8,-C9,-C10,-C11,-C12,-C13,-C14)</f>
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="13" t="s">
@@ -864,7 +879,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D16" s="3"/>
       <c r="E16" s="6" t="s">
         <v>31</v>
@@ -873,7 +888,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="15.75" customHeight="1">
+    <row r="17" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D17" s="3"/>
       <c r="E17" s="6" t="s">
         <v>32</v>
@@ -882,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:7" ht="15.75" customHeight="1">
+    <row r="18" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D18" s="3"/>
       <c r="E18" s="8" t="s">
         <v>33</v>
@@ -890,7 +905,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="4:7" ht="15.75" customHeight="1">
+    <row r="19" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D19" s="3"/>
       <c r="E19" s="13" t="s">
         <v>34</v>
@@ -899,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:7" ht="15.75" customHeight="1">
+    <row r="20" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D20" s="3"/>
       <c r="E20" s="13" t="s">
         <v>35</v>
@@ -908,7 +923,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="21" spans="4:7" ht="15.75" customHeight="1">
+    <row r="21" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D21" s="3"/>
       <c r="E21" s="13" t="s">
         <v>36</v>
@@ -917,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:7" ht="15.75" customHeight="1">
+    <row r="22" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D22" s="3"/>
       <c r="E22" s="8" t="s">
         <v>37</v>
@@ -925,7 +940,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="4:7" ht="15.75" customHeight="1">
+    <row r="23" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D23" s="3"/>
       <c r="E23" s="13" t="s">
         <v>38</v>
@@ -934,7 +949,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="24" spans="4:7" ht="15.75" customHeight="1">
+    <row r="24" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D24" s="3"/>
       <c r="E24" s="13" t="s">
         <v>39</v>
@@ -943,7 +958,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="25" spans="4:7" ht="15.75" customHeight="1">
+    <row r="25" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D25" s="3"/>
       <c r="E25" s="6" t="s">
         <v>40</v>
@@ -953,7 +968,7 @@
         <v>1638.4</v>
       </c>
     </row>
-    <row r="26" spans="4:7" ht="15.75" customHeight="1">
+    <row r="26" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D26" s="3"/>
       <c r="E26" s="6" t="s">
         <v>41</v>
@@ -963,2948 +978,2943 @@
         <v>3276.8</v>
       </c>
     </row>
-    <row r="27" spans="4:7" ht="15.75" customHeight="1">
+    <row r="27" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D27" s="3"/>
       <c r="E27" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="11">
         <f>MIN(G12,G14,PRODUCT(B4,B5))</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D28" s="3"/>
       <c r="E28" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F28" s="11">
         <f>MIN(G12,G14,PRODUCT(B4,B5))</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="4:7" ht="15.75" customHeight="1">
+    <row r="30" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="4:7" ht="15.75" customHeight="1">
+    <row r="31" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="4:7" ht="15.75" customHeight="1">
+    <row r="32" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="4:4" ht="15.75" customHeight="1">
+    <row r="33" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="4:4" ht="15.75" customHeight="1">
+    <row r="34" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="4:4" ht="15.75" customHeight="1">
+    <row r="35" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="4:4" ht="15.75" customHeight="1">
+    <row r="36" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="4:4" ht="15.75" customHeight="1">
+    <row r="37" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="4:4" ht="15.75" customHeight="1">
+    <row r="38" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="4:4" ht="15.75" customHeight="1">
+    <row r="39" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="4:4" ht="15.75" customHeight="1">
+    <row r="40" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="4:4" ht="15.75" customHeight="1">
+    <row r="41" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="4:4" ht="15.75" customHeight="1">
+    <row r="42" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="4:4" ht="15.75" customHeight="1">
+    <row r="43" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="4:4" ht="15.75" customHeight="1">
+    <row r="44" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="4:4" ht="15.75" customHeight="1">
+    <row r="45" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="4:4" ht="15.75" customHeight="1">
+    <row r="46" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="4:4" ht="15.75" customHeight="1">
+    <row r="47" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="4:4" ht="15.75" customHeight="1">
+    <row r="48" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4" ht="15.75" customHeight="1">
+    <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="4:4" ht="15.75" customHeight="1">
+    <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="4:4" ht="15.75" customHeight="1">
+    <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="4:4" ht="15.75" customHeight="1">
+    <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="4:4" ht="15.75" customHeight="1">
+    <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="4:4" ht="15.75" customHeight="1">
+    <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="4:4" ht="15.75" customHeight="1">
+    <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="4:4" ht="15.75" customHeight="1">
+    <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="4:4" ht="15.75" customHeight="1">
+    <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="4:4" ht="15.75" customHeight="1">
+    <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="4:4" ht="15.75" customHeight="1">
+    <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="4:4" ht="15.75" customHeight="1">
+    <row r="60" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="4:4" ht="15.75" customHeight="1">
+    <row r="61" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="4:4" ht="15.75" customHeight="1">
+    <row r="62" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="4:4" ht="15.75" customHeight="1">
+    <row r="63" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="4:4" ht="15.75" customHeight="1">
+    <row r="64" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="4:4" ht="15.75" customHeight="1">
+    <row r="65" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="4:4" ht="15.75" customHeight="1">
+    <row r="66" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="4:4" ht="15.75" customHeight="1">
+    <row r="67" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="4:4" ht="15.75" customHeight="1">
+    <row r="68" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="4:4" ht="15.75" customHeight="1">
+    <row r="69" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="4:4" ht="15.75" customHeight="1">
+    <row r="70" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="4:4" ht="15.75" customHeight="1">
+    <row r="71" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="4:4" ht="15.75" customHeight="1">
+    <row r="72" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="4:4" ht="15.75" customHeight="1">
+    <row r="73" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="4:4" ht="15.75" customHeight="1">
+    <row r="74" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="4:4" ht="15.75" customHeight="1">
+    <row r="75" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="4:4" ht="15.75" customHeight="1">
+    <row r="76" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="4:4" ht="15.75" customHeight="1">
+    <row r="77" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="4:4" ht="15.75" customHeight="1">
+    <row r="78" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="4:4" ht="15.75" customHeight="1">
+    <row r="79" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="4:4" ht="15.75" customHeight="1">
+    <row r="80" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="4:4" ht="15.75" customHeight="1">
+    <row r="81" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="4:4" ht="15.75" customHeight="1">
+    <row r="82" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="4:4" ht="15.75" customHeight="1">
+    <row r="83" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="4:4" ht="15.75" customHeight="1">
+    <row r="84" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="4:4" ht="15.75" customHeight="1">
+    <row r="85" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="4:4" ht="15.75" customHeight="1">
+    <row r="86" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="4:4" ht="15.75" customHeight="1">
+    <row r="87" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="4:4" ht="15.75" customHeight="1">
+    <row r="88" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="4:4" ht="15.75" customHeight="1">
+    <row r="89" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="4:4" ht="15.75" customHeight="1">
+    <row r="90" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="4:4" ht="15.75" customHeight="1">
+    <row r="91" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="4:4" ht="15.75" customHeight="1">
+    <row r="92" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="4:4" ht="15.75" customHeight="1">
+    <row r="93" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="4:4" ht="15.75" customHeight="1">
+    <row r="94" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="4:4" ht="15.75" customHeight="1">
+    <row r="95" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="4:4" ht="15.75" customHeight="1">
+    <row r="96" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="4:4" ht="15.75" customHeight="1">
+    <row r="97" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="4:4" ht="15.75" customHeight="1">
+    <row r="98" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="4:4" ht="15.75" customHeight="1">
+    <row r="99" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="4:4" ht="15.75" customHeight="1">
+    <row r="100" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="4:4" ht="15.75" customHeight="1">
+    <row r="101" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="4:4" ht="15.75" customHeight="1">
+    <row r="102" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="4:4" ht="15.75" customHeight="1">
+    <row r="103" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="4:4" ht="15.75" customHeight="1">
+    <row r="104" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="4:4" ht="15.75" customHeight="1">
+    <row r="105" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="4:4" ht="15.75" customHeight="1">
+    <row r="106" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="4:4" ht="15.75" customHeight="1">
+    <row r="107" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="4:4" ht="15.75" customHeight="1">
+    <row r="108" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="4:4" ht="15.75" customHeight="1">
+    <row r="109" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="4:4" ht="15.75" customHeight="1">
+    <row r="110" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="4:4" ht="15.75" customHeight="1">
+    <row r="111" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="4:4" ht="15.75" customHeight="1">
+    <row r="112" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="4:4" ht="15.75" customHeight="1">
+    <row r="113" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="4:4" ht="15.75" customHeight="1">
+    <row r="114" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="4:4" ht="15.75" customHeight="1">
+    <row r="115" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="4:4" ht="15.75" customHeight="1">
+    <row r="116" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="4:4" ht="15.75" customHeight="1">
+    <row r="117" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="4:4" ht="15.75" customHeight="1">
+    <row r="118" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="4:4" ht="15.75" customHeight="1">
+    <row r="119" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="4:4" ht="15.75" customHeight="1">
+    <row r="120" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="4:4" ht="15.75" customHeight="1">
+    <row r="121" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="4:4" ht="15.75" customHeight="1">
+    <row r="122" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="4:4" ht="15.75" customHeight="1">
+    <row r="123" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="4:4" ht="15.75" customHeight="1">
+    <row r="124" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="4:4" ht="15.75" customHeight="1">
+    <row r="125" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="4:4" ht="15.75" customHeight="1">
+    <row r="126" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="4:4" ht="15.75" customHeight="1">
+    <row r="127" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="4:4" ht="15.75" customHeight="1">
+    <row r="128" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="4:4" ht="15.75" customHeight="1">
+    <row r="129" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D129" s="3"/>
     </row>
-    <row r="130" spans="4:4" ht="15.75" customHeight="1">
+    <row r="130" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="4:4" ht="15.75" customHeight="1">
+    <row r="131" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="4:4" ht="15.75" customHeight="1">
+    <row r="132" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="4:4" ht="15.75" customHeight="1">
+    <row r="133" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="4:4" ht="15.75" customHeight="1">
+    <row r="134" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="4:4" ht="15.75" customHeight="1">
+    <row r="135" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="4:4" ht="15.75" customHeight="1">
+    <row r="136" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="4:4" ht="15.75" customHeight="1">
+    <row r="137" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D137" s="3"/>
     </row>
-    <row r="138" spans="4:4" ht="15.75" customHeight="1">
+    <row r="138" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="4:4" ht="15.75" customHeight="1">
+    <row r="139" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="4:4" ht="15.75" customHeight="1">
+    <row r="140" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="4:4" ht="15.75" customHeight="1">
+    <row r="141" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="4:4" ht="15.75" customHeight="1">
+    <row r="142" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D142" s="3"/>
     </row>
-    <row r="143" spans="4:4" ht="15.75" customHeight="1">
+    <row r="143" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D143" s="3"/>
     </row>
-    <row r="144" spans="4:4" ht="15.75" customHeight="1">
+    <row r="144" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="4:4" ht="15.75" customHeight="1">
+    <row r="145" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="4:4" ht="15.75" customHeight="1">
+    <row r="146" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="4:4" ht="15.75" customHeight="1">
+    <row r="147" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="4:4" ht="15.75" customHeight="1">
+    <row r="148" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="4:4" ht="15.75" customHeight="1">
+    <row r="149" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="4:4" ht="15.75" customHeight="1">
+    <row r="150" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="4:4" ht="15.75" customHeight="1">
+    <row r="151" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D151" s="3"/>
     </row>
-    <row r="152" spans="4:4" ht="15.75" customHeight="1">
+    <row r="152" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D152" s="3"/>
     </row>
-    <row r="153" spans="4:4" ht="15.75" customHeight="1">
+    <row r="153" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D153" s="3"/>
     </row>
-    <row r="154" spans="4:4" ht="15.75" customHeight="1">
+    <row r="154" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="4:4" ht="15.75" customHeight="1">
+    <row r="155" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D155" s="3"/>
     </row>
-    <row r="156" spans="4:4" ht="15.75" customHeight="1">
+    <row r="156" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D156" s="3"/>
     </row>
-    <row r="157" spans="4:4" ht="15.75" customHeight="1">
+    <row r="157" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D157" s="3"/>
     </row>
-    <row r="158" spans="4:4" ht="15.75" customHeight="1">
+    <row r="158" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D158" s="3"/>
     </row>
-    <row r="159" spans="4:4" ht="15.75" customHeight="1">
+    <row r="159" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D159" s="3"/>
     </row>
-    <row r="160" spans="4:4" ht="15.75" customHeight="1">
+    <row r="160" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D160" s="3"/>
     </row>
-    <row r="161" spans="4:4" ht="15.75" customHeight="1">
+    <row r="161" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D161" s="3"/>
     </row>
-    <row r="162" spans="4:4" ht="15.75" customHeight="1">
+    <row r="162" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D162" s="3"/>
     </row>
-    <row r="163" spans="4:4" ht="15.75" customHeight="1">
+    <row r="163" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D163" s="3"/>
     </row>
-    <row r="164" spans="4:4" ht="15.75" customHeight="1">
+    <row r="164" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D164" s="3"/>
     </row>
-    <row r="165" spans="4:4" ht="15.75" customHeight="1">
+    <row r="165" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D165" s="3"/>
     </row>
-    <row r="166" spans="4:4" ht="15.75" customHeight="1">
+    <row r="166" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D166" s="3"/>
     </row>
-    <row r="167" spans="4:4" ht="15.75" customHeight="1">
+    <row r="167" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D167" s="3"/>
     </row>
-    <row r="168" spans="4:4" ht="15.75" customHeight="1">
+    <row r="168" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D168" s="3"/>
     </row>
-    <row r="169" spans="4:4" ht="15.75" customHeight="1">
+    <row r="169" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D169" s="3"/>
     </row>
-    <row r="170" spans="4:4" ht="15.75" customHeight="1">
+    <row r="170" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D170" s="3"/>
     </row>
-    <row r="171" spans="4:4" ht="15.75" customHeight="1">
+    <row r="171" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D171" s="3"/>
     </row>
-    <row r="172" spans="4:4" ht="15.75" customHeight="1">
+    <row r="172" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D172" s="3"/>
     </row>
-    <row r="173" spans="4:4" ht="15.75" customHeight="1">
+    <row r="173" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D173" s="3"/>
     </row>
-    <row r="174" spans="4:4" ht="15.75" customHeight="1">
+    <row r="174" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D174" s="3"/>
     </row>
-    <row r="175" spans="4:4" ht="15.75" customHeight="1">
+    <row r="175" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D175" s="3"/>
     </row>
-    <row r="176" spans="4:4" ht="15.75" customHeight="1">
+    <row r="176" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D176" s="3"/>
     </row>
-    <row r="177" spans="4:4" ht="15.75" customHeight="1">
+    <row r="177" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D177" s="3"/>
     </row>
-    <row r="178" spans="4:4" ht="15.75" customHeight="1">
+    <row r="178" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D178" s="3"/>
     </row>
-    <row r="179" spans="4:4" ht="15.75" customHeight="1">
+    <row r="179" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D179" s="3"/>
     </row>
-    <row r="180" spans="4:4" ht="15.75" customHeight="1">
+    <row r="180" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D180" s="3"/>
     </row>
-    <row r="181" spans="4:4" ht="15.75" customHeight="1">
+    <row r="181" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D181" s="3"/>
     </row>
-    <row r="182" spans="4:4" ht="15.75" customHeight="1">
+    <row r="182" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D182" s="3"/>
     </row>
-    <row r="183" spans="4:4" ht="15.75" customHeight="1">
+    <row r="183" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D183" s="3"/>
     </row>
-    <row r="184" spans="4:4" ht="15.75" customHeight="1">
+    <row r="184" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D184" s="3"/>
     </row>
-    <row r="185" spans="4:4" ht="15.75" customHeight="1">
+    <row r="185" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D185" s="3"/>
     </row>
-    <row r="186" spans="4:4" ht="15.75" customHeight="1">
+    <row r="186" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D186" s="3"/>
     </row>
-    <row r="187" spans="4:4" ht="15.75" customHeight="1">
+    <row r="187" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D187" s="3"/>
     </row>
-    <row r="188" spans="4:4" ht="15.75" customHeight="1">
+    <row r="188" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D188" s="3"/>
     </row>
-    <row r="189" spans="4:4" ht="15.75" customHeight="1">
+    <row r="189" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D189" s="3"/>
     </row>
-    <row r="190" spans="4:4" ht="15.75" customHeight="1">
+    <row r="190" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D190" s="3"/>
     </row>
-    <row r="191" spans="4:4" ht="15.75" customHeight="1">
+    <row r="191" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D191" s="3"/>
     </row>
-    <row r="192" spans="4:4" ht="15.75" customHeight="1">
+    <row r="192" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D192" s="3"/>
     </row>
-    <row r="193" spans="4:4" ht="15.75" customHeight="1">
+    <row r="193" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D193" s="3"/>
     </row>
-    <row r="194" spans="4:4" ht="15.75" customHeight="1">
+    <row r="194" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D194" s="3"/>
     </row>
-    <row r="195" spans="4:4" ht="15.75" customHeight="1">
+    <row r="195" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D195" s="3"/>
     </row>
-    <row r="196" spans="4:4" ht="15.75" customHeight="1">
+    <row r="196" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D196" s="3"/>
     </row>
-    <row r="197" spans="4:4" ht="15.75" customHeight="1">
+    <row r="197" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="4:4" ht="15.75" customHeight="1">
+    <row r="198" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D198" s="3"/>
     </row>
-    <row r="199" spans="4:4" ht="15.75" customHeight="1">
+    <row r="199" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="4:4" ht="15.75" customHeight="1">
+    <row r="200" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D200" s="3"/>
     </row>
-    <row r="201" spans="4:4" ht="15.75" customHeight="1">
+    <row r="201" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="4:4" ht="15.75" customHeight="1">
+    <row r="202" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D202" s="3"/>
     </row>
-    <row r="203" spans="4:4" ht="15.75" customHeight="1">
+    <row r="203" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D203" s="3"/>
     </row>
-    <row r="204" spans="4:4" ht="15.75" customHeight="1">
+    <row r="204" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D204" s="3"/>
     </row>
-    <row r="205" spans="4:4" ht="15.75" customHeight="1">
+    <row r="205" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="4:4" ht="15.75" customHeight="1">
+    <row r="206" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="4:4" ht="15.75" customHeight="1">
+    <row r="207" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D207" s="3"/>
     </row>
-    <row r="208" spans="4:4" ht="15.75" customHeight="1">
+    <row r="208" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D208" s="3"/>
     </row>
-    <row r="209" spans="4:4" ht="15.75" customHeight="1">
+    <row r="209" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D209" s="3"/>
     </row>
-    <row r="210" spans="4:4" ht="15.75" customHeight="1">
+    <row r="210" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D210" s="3"/>
     </row>
-    <row r="211" spans="4:4" ht="15.75" customHeight="1">
+    <row r="211" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D211" s="3"/>
     </row>
-    <row r="212" spans="4:4" ht="15.75" customHeight="1">
+    <row r="212" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D212" s="3"/>
     </row>
-    <row r="213" spans="4:4" ht="15.75" customHeight="1">
+    <row r="213" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D213" s="3"/>
     </row>
-    <row r="214" spans="4:4" ht="15.75" customHeight="1">
+    <row r="214" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="4:4" ht="15.75" customHeight="1">
+    <row r="215" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D215" s="3"/>
     </row>
-    <row r="216" spans="4:4" ht="15.75" customHeight="1">
+    <row r="216" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D216" s="3"/>
     </row>
-    <row r="217" spans="4:4" ht="15.75" customHeight="1">
+    <row r="217" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D217" s="3"/>
     </row>
-    <row r="218" spans="4:4" ht="15.75" customHeight="1">
+    <row r="218" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="4:4" ht="15.75" customHeight="1">
+    <row r="219" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="4:4" ht="15.75" customHeight="1">
+    <row r="220" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D220" s="3"/>
     </row>
-    <row r="221" spans="4:4" ht="15.75" customHeight="1">
+    <row r="221" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D221" s="3"/>
     </row>
-    <row r="222" spans="4:4" ht="15.75" customHeight="1">
+    <row r="222" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D222" s="3"/>
     </row>
-    <row r="223" spans="4:4" ht="15.75" customHeight="1">
+    <row r="223" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D223" s="3"/>
     </row>
-    <row r="224" spans="4:4" ht="15.75" customHeight="1">
+    <row r="224" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D224" s="3"/>
     </row>
-    <row r="225" spans="4:4" ht="15.75" customHeight="1">
+    <row r="225" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D225" s="3"/>
     </row>
-    <row r="226" spans="4:4" ht="15.75" customHeight="1">
+    <row r="226" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D226" s="3"/>
     </row>
-    <row r="227" spans="4:4" ht="15.75" customHeight="1">
+    <row r="227" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D227" s="3"/>
     </row>
-    <row r="228" spans="4:4" ht="15.75" customHeight="1">
+    <row r="228" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D228" s="3"/>
     </row>
-    <row r="229" spans="4:4" ht="15.75" customHeight="1">
+    <row r="229" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D229" s="3"/>
     </row>
-    <row r="230" spans="4:4" ht="15.75" customHeight="1">
+    <row r="230" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D230" s="3"/>
     </row>
-    <row r="231" spans="4:4" ht="15.75" customHeight="1">
+    <row r="231" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D231" s="3"/>
     </row>
-    <row r="232" spans="4:4" ht="15.75" customHeight="1">
+    <row r="232" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D232" s="3"/>
     </row>
-    <row r="233" spans="4:4" ht="15.75" customHeight="1">
+    <row r="233" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D233" s="3"/>
     </row>
-    <row r="234" spans="4:4" ht="15.75" customHeight="1">
+    <row r="234" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D234" s="3"/>
     </row>
-    <row r="235" spans="4:4" ht="15.75" customHeight="1">
+    <row r="235" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D235" s="3"/>
     </row>
-    <row r="236" spans="4:4" ht="15.75" customHeight="1">
+    <row r="236" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D236" s="3"/>
     </row>
-    <row r="237" spans="4:4" ht="15.75" customHeight="1">
+    <row r="237" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D237" s="3"/>
     </row>
-    <row r="238" spans="4:4" ht="15.75" customHeight="1">
+    <row r="238" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D238" s="3"/>
     </row>
-    <row r="239" spans="4:4" ht="15.75" customHeight="1">
+    <row r="239" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D239" s="3"/>
     </row>
-    <row r="240" spans="4:4" ht="15.75" customHeight="1">
+    <row r="240" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D240" s="3"/>
     </row>
-    <row r="241" spans="4:4" ht="15.75" customHeight="1">
+    <row r="241" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D241" s="3"/>
     </row>
-    <row r="242" spans="4:4" ht="15.75" customHeight="1">
+    <row r="242" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D242" s="3"/>
     </row>
-    <row r="243" spans="4:4" ht="15.75" customHeight="1">
+    <row r="243" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D243" s="3"/>
     </row>
-    <row r="244" spans="4:4" ht="15.75" customHeight="1">
+    <row r="244" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D244" s="3"/>
     </row>
-    <row r="245" spans="4:4" ht="15.75" customHeight="1">
+    <row r="245" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D245" s="3"/>
     </row>
-    <row r="246" spans="4:4" ht="15.75" customHeight="1">
+    <row r="246" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D246" s="3"/>
     </row>
-    <row r="247" spans="4:4" ht="15.75" customHeight="1">
+    <row r="247" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D247" s="3"/>
     </row>
-    <row r="248" spans="4:4" ht="15.75" customHeight="1">
+    <row r="248" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D248" s="3"/>
     </row>
-    <row r="249" spans="4:4" ht="15.75" customHeight="1">
+    <row r="249" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D249" s="3"/>
     </row>
-    <row r="250" spans="4:4" ht="15.75" customHeight="1">
+    <row r="250" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="4:4" ht="15.75" customHeight="1">
+    <row r="251" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D251" s="3"/>
     </row>
-    <row r="252" spans="4:4" ht="15.75" customHeight="1">
+    <row r="252" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D252" s="3"/>
     </row>
-    <row r="253" spans="4:4" ht="15.75" customHeight="1">
+    <row r="253" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D253" s="3"/>
     </row>
-    <row r="254" spans="4:4" ht="15.75" customHeight="1">
+    <row r="254" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D254" s="3"/>
     </row>
-    <row r="255" spans="4:4" ht="15.75" customHeight="1">
+    <row r="255" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D255" s="3"/>
     </row>
-    <row r="256" spans="4:4" ht="15.75" customHeight="1">
+    <row r="256" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D256" s="3"/>
     </row>
-    <row r="257" spans="4:4" ht="15.75" customHeight="1">
+    <row r="257" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D257" s="3"/>
     </row>
-    <row r="258" spans="4:4" ht="15.75" customHeight="1">
+    <row r="258" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D258" s="3"/>
     </row>
-    <row r="259" spans="4:4" ht="15.75" customHeight="1">
+    <row r="259" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D259" s="3"/>
     </row>
-    <row r="260" spans="4:4" ht="15.75" customHeight="1">
+    <row r="260" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D260" s="3"/>
     </row>
-    <row r="261" spans="4:4" ht="15.75" customHeight="1">
+    <row r="261" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D261" s="3"/>
     </row>
-    <row r="262" spans="4:4" ht="15.75" customHeight="1">
+    <row r="262" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D262" s="3"/>
     </row>
-    <row r="263" spans="4:4" ht="15.75" customHeight="1">
+    <row r="263" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D263" s="3"/>
     </row>
-    <row r="264" spans="4:4" ht="15.75" customHeight="1">
+    <row r="264" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D264" s="3"/>
     </row>
-    <row r="265" spans="4:4" ht="15.75" customHeight="1">
+    <row r="265" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D265" s="3"/>
     </row>
-    <row r="266" spans="4:4" ht="15.75" customHeight="1">
+    <row r="266" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D266" s="3"/>
     </row>
-    <row r="267" spans="4:4" ht="15.75" customHeight="1">
+    <row r="267" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D267" s="3"/>
     </row>
-    <row r="268" spans="4:4" ht="15.75" customHeight="1">
+    <row r="268" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D268" s="3"/>
     </row>
-    <row r="269" spans="4:4" ht="15.75" customHeight="1">
+    <row r="269" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D269" s="3"/>
     </row>
-    <row r="270" spans="4:4" ht="15.75" customHeight="1">
+    <row r="270" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D270" s="3"/>
     </row>
-    <row r="271" spans="4:4" ht="15.75" customHeight="1">
+    <row r="271" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D271" s="3"/>
     </row>
-    <row r="272" spans="4:4" ht="15.75" customHeight="1">
+    <row r="272" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D272" s="3"/>
     </row>
-    <row r="273" spans="4:4" ht="15.75" customHeight="1">
+    <row r="273" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D273" s="3"/>
     </row>
-    <row r="274" spans="4:4" ht="15.75" customHeight="1">
+    <row r="274" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D274" s="3"/>
     </row>
-    <row r="275" spans="4:4" ht="15.75" customHeight="1">
+    <row r="275" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D275" s="3"/>
     </row>
-    <row r="276" spans="4:4" ht="15.75" customHeight="1">
+    <row r="276" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D276" s="3"/>
     </row>
-    <row r="277" spans="4:4" ht="15.75" customHeight="1">
+    <row r="277" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D277" s="3"/>
     </row>
-    <row r="278" spans="4:4" ht="15.75" customHeight="1">
+    <row r="278" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D278" s="3"/>
     </row>
-    <row r="279" spans="4:4" ht="15.75" customHeight="1">
+    <row r="279" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D279" s="3"/>
     </row>
-    <row r="280" spans="4:4" ht="15.75" customHeight="1">
+    <row r="280" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D280" s="3"/>
     </row>
-    <row r="281" spans="4:4" ht="15.75" customHeight="1">
+    <row r="281" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D281" s="3"/>
     </row>
-    <row r="282" spans="4:4" ht="15.75" customHeight="1">
+    <row r="282" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D282" s="3"/>
     </row>
-    <row r="283" spans="4:4" ht="15.75" customHeight="1">
+    <row r="283" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D283" s="3"/>
     </row>
-    <row r="284" spans="4:4" ht="15.75" customHeight="1">
+    <row r="284" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D284" s="3"/>
     </row>
-    <row r="285" spans="4:4" ht="15.75" customHeight="1">
+    <row r="285" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D285" s="3"/>
     </row>
-    <row r="286" spans="4:4" ht="15.75" customHeight="1">
+    <row r="286" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D286" s="3"/>
     </row>
-    <row r="287" spans="4:4" ht="15.75" customHeight="1">
+    <row r="287" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D287" s="3"/>
     </row>
-    <row r="288" spans="4:4" ht="15.75" customHeight="1">
+    <row r="288" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D288" s="3"/>
     </row>
-    <row r="289" spans="4:4" ht="15.75" customHeight="1">
+    <row r="289" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D289" s="3"/>
     </row>
-    <row r="290" spans="4:4" ht="15.75" customHeight="1">
+    <row r="290" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D290" s="3"/>
     </row>
-    <row r="291" spans="4:4" ht="15.75" customHeight="1">
+    <row r="291" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D291" s="3"/>
     </row>
-    <row r="292" spans="4:4" ht="15.75" customHeight="1">
+    <row r="292" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D292" s="3"/>
     </row>
-    <row r="293" spans="4:4" ht="15.75" customHeight="1">
+    <row r="293" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D293" s="3"/>
     </row>
-    <row r="294" spans="4:4" ht="15.75" customHeight="1">
+    <row r="294" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D294" s="3"/>
     </row>
-    <row r="295" spans="4:4" ht="15.75" customHeight="1">
+    <row r="295" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D295" s="3"/>
     </row>
-    <row r="296" spans="4:4" ht="15.75" customHeight="1">
+    <row r="296" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D296" s="3"/>
     </row>
-    <row r="297" spans="4:4" ht="15.75" customHeight="1">
+    <row r="297" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D297" s="3"/>
     </row>
-    <row r="298" spans="4:4" ht="15.75" customHeight="1">
+    <row r="298" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D298" s="3"/>
     </row>
-    <row r="299" spans="4:4" ht="15.75" customHeight="1">
+    <row r="299" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D299" s="3"/>
     </row>
-    <row r="300" spans="4:4" ht="15.75" customHeight="1">
+    <row r="300" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D300" s="3"/>
     </row>
-    <row r="301" spans="4:4" ht="15.75" customHeight="1">
+    <row r="301" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D301" s="3"/>
     </row>
-    <row r="302" spans="4:4" ht="15.75" customHeight="1">
+    <row r="302" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D302" s="3"/>
     </row>
-    <row r="303" spans="4:4" ht="15.75" customHeight="1">
+    <row r="303" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D303" s="3"/>
     </row>
-    <row r="304" spans="4:4" ht="15.75" customHeight="1">
+    <row r="304" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D304" s="3"/>
     </row>
-    <row r="305" spans="4:4" ht="15.75" customHeight="1">
+    <row r="305" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D305" s="3"/>
     </row>
-    <row r="306" spans="4:4" ht="15.75" customHeight="1">
+    <row r="306" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D306" s="3"/>
     </row>
-    <row r="307" spans="4:4" ht="15.75" customHeight="1">
+    <row r="307" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D307" s="3"/>
     </row>
-    <row r="308" spans="4:4" ht="15.75" customHeight="1">
+    <row r="308" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D308" s="3"/>
     </row>
-    <row r="309" spans="4:4" ht="15.75" customHeight="1">
+    <row r="309" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D309" s="3"/>
     </row>
-    <row r="310" spans="4:4" ht="15.75" customHeight="1">
+    <row r="310" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D310" s="3"/>
     </row>
-    <row r="311" spans="4:4" ht="15.75" customHeight="1">
+    <row r="311" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D311" s="3"/>
     </row>
-    <row r="312" spans="4:4" ht="15.75" customHeight="1">
+    <row r="312" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D312" s="3"/>
     </row>
-    <row r="313" spans="4:4" ht="15.75" customHeight="1">
+    <row r="313" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D313" s="3"/>
     </row>
-    <row r="314" spans="4:4" ht="15.75" customHeight="1">
+    <row r="314" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D314" s="3"/>
     </row>
-    <row r="315" spans="4:4" ht="15.75" customHeight="1">
+    <row r="315" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D315" s="3"/>
     </row>
-    <row r="316" spans="4:4" ht="15.75" customHeight="1">
+    <row r="316" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D316" s="3"/>
     </row>
-    <row r="317" spans="4:4" ht="15.75" customHeight="1">
+    <row r="317" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D317" s="3"/>
     </row>
-    <row r="318" spans="4:4" ht="15.75" customHeight="1">
+    <row r="318" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D318" s="3"/>
     </row>
-    <row r="319" spans="4:4" ht="15.75" customHeight="1">
+    <row r="319" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D319" s="3"/>
     </row>
-    <row r="320" spans="4:4" ht="15.75" customHeight="1">
+    <row r="320" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D320" s="3"/>
     </row>
-    <row r="321" spans="4:4" ht="15.75" customHeight="1">
+    <row r="321" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D321" s="3"/>
     </row>
-    <row r="322" spans="4:4" ht="15.75" customHeight="1">
+    <row r="322" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D322" s="3"/>
     </row>
-    <row r="323" spans="4:4" ht="15.75" customHeight="1">
+    <row r="323" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D323" s="3"/>
     </row>
-    <row r="324" spans="4:4" ht="15.75" customHeight="1">
+    <row r="324" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D324" s="3"/>
     </row>
-    <row r="325" spans="4:4" ht="15.75" customHeight="1">
+    <row r="325" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D325" s="3"/>
     </row>
-    <row r="326" spans="4:4" ht="15.75" customHeight="1">
+    <row r="326" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D326" s="3"/>
     </row>
-    <row r="327" spans="4:4" ht="15.75" customHeight="1">
+    <row r="327" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D327" s="3"/>
     </row>
-    <row r="328" spans="4:4" ht="15.75" customHeight="1">
+    <row r="328" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D328" s="3"/>
     </row>
-    <row r="329" spans="4:4" ht="15.75" customHeight="1">
+    <row r="329" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D329" s="3"/>
     </row>
-    <row r="330" spans="4:4" ht="15.75" customHeight="1">
+    <row r="330" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D330" s="3"/>
     </row>
-    <row r="331" spans="4:4" ht="15.75" customHeight="1">
+    <row r="331" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D331" s="3"/>
     </row>
-    <row r="332" spans="4:4" ht="15.75" customHeight="1">
+    <row r="332" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D332" s="3"/>
     </row>
-    <row r="333" spans="4:4" ht="15.75" customHeight="1">
+    <row r="333" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D333" s="3"/>
     </row>
-    <row r="334" spans="4:4" ht="15.75" customHeight="1">
+    <row r="334" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D334" s="3"/>
     </row>
-    <row r="335" spans="4:4" ht="15.75" customHeight="1">
+    <row r="335" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D335" s="3"/>
     </row>
-    <row r="336" spans="4:4" ht="15.75" customHeight="1">
+    <row r="336" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D336" s="3"/>
     </row>
-    <row r="337" spans="4:4" ht="15.75" customHeight="1">
+    <row r="337" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D337" s="3"/>
     </row>
-    <row r="338" spans="4:4" ht="15.75" customHeight="1">
+    <row r="338" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D338" s="3"/>
     </row>
-    <row r="339" spans="4:4" ht="15.75" customHeight="1">
+    <row r="339" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D339" s="3"/>
     </row>
-    <row r="340" spans="4:4" ht="15.75" customHeight="1">
+    <row r="340" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D340" s="3"/>
     </row>
-    <row r="341" spans="4:4" ht="15.75" customHeight="1">
+    <row r="341" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D341" s="3"/>
     </row>
-    <row r="342" spans="4:4" ht="15.75" customHeight="1">
+    <row r="342" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D342" s="3"/>
     </row>
-    <row r="343" spans="4:4" ht="15.75" customHeight="1">
+    <row r="343" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D343" s="3"/>
     </row>
-    <row r="344" spans="4:4" ht="15.75" customHeight="1">
+    <row r="344" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D344" s="3"/>
     </row>
-    <row r="345" spans="4:4" ht="15.75" customHeight="1">
+    <row r="345" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D345" s="3"/>
     </row>
-    <row r="346" spans="4:4" ht="15.75" customHeight="1">
+    <row r="346" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D346" s="3"/>
     </row>
-    <row r="347" spans="4:4" ht="15.75" customHeight="1">
+    <row r="347" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D347" s="3"/>
     </row>
-    <row r="348" spans="4:4" ht="15.75" customHeight="1">
+    <row r="348" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D348" s="3"/>
     </row>
-    <row r="349" spans="4:4" ht="15.75" customHeight="1">
+    <row r="349" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D349" s="3"/>
     </row>
-    <row r="350" spans="4:4" ht="15.75" customHeight="1">
+    <row r="350" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D350" s="3"/>
     </row>
-    <row r="351" spans="4:4" ht="15.75" customHeight="1">
+    <row r="351" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D351" s="3"/>
     </row>
-    <row r="352" spans="4:4" ht="15.75" customHeight="1">
+    <row r="352" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D352" s="3"/>
     </row>
-    <row r="353" spans="4:4" ht="15.75" customHeight="1">
+    <row r="353" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D353" s="3"/>
     </row>
-    <row r="354" spans="4:4" ht="15.75" customHeight="1">
+    <row r="354" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D354" s="3"/>
     </row>
-    <row r="355" spans="4:4" ht="15.75" customHeight="1">
+    <row r="355" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D355" s="3"/>
     </row>
-    <row r="356" spans="4:4" ht="15.75" customHeight="1">
+    <row r="356" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D356" s="3"/>
     </row>
-    <row r="357" spans="4:4" ht="15.75" customHeight="1">
+    <row r="357" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D357" s="3"/>
     </row>
-    <row r="358" spans="4:4" ht="15.75" customHeight="1">
+    <row r="358" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D358" s="3"/>
     </row>
-    <row r="359" spans="4:4" ht="15.75" customHeight="1">
+    <row r="359" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D359" s="3"/>
     </row>
-    <row r="360" spans="4:4" ht="15.75" customHeight="1">
+    <row r="360" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D360" s="3"/>
     </row>
-    <row r="361" spans="4:4" ht="15.75" customHeight="1">
+    <row r="361" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D361" s="3"/>
     </row>
-    <row r="362" spans="4:4" ht="15.75" customHeight="1">
+    <row r="362" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D362" s="3"/>
     </row>
-    <row r="363" spans="4:4" ht="15.75" customHeight="1">
+    <row r="363" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D363" s="3"/>
     </row>
-    <row r="364" spans="4:4" ht="15.75" customHeight="1">
+    <row r="364" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D364" s="3"/>
     </row>
-    <row r="365" spans="4:4" ht="15.75" customHeight="1">
+    <row r="365" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D365" s="3"/>
     </row>
-    <row r="366" spans="4:4" ht="15.75" customHeight="1">
+    <row r="366" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D366" s="3"/>
     </row>
-    <row r="367" spans="4:4" ht="15.75" customHeight="1">
+    <row r="367" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D367" s="3"/>
     </row>
-    <row r="368" spans="4:4" ht="15.75" customHeight="1">
+    <row r="368" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D368" s="3"/>
     </row>
-    <row r="369" spans="4:4" ht="15.75" customHeight="1">
+    <row r="369" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D369" s="3"/>
     </row>
-    <row r="370" spans="4:4" ht="15.75" customHeight="1">
+    <row r="370" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D370" s="3"/>
     </row>
-    <row r="371" spans="4:4" ht="15.75" customHeight="1">
+    <row r="371" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D371" s="3"/>
     </row>
-    <row r="372" spans="4:4" ht="15.75" customHeight="1">
+    <row r="372" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D372" s="3"/>
     </row>
-    <row r="373" spans="4:4" ht="15.75" customHeight="1">
+    <row r="373" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D373" s="3"/>
     </row>
-    <row r="374" spans="4:4" ht="15.75" customHeight="1">
+    <row r="374" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D374" s="3"/>
     </row>
-    <row r="375" spans="4:4" ht="15.75" customHeight="1">
+    <row r="375" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D375" s="3"/>
     </row>
-    <row r="376" spans="4:4" ht="15.75" customHeight="1">
+    <row r="376" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D376" s="3"/>
     </row>
-    <row r="377" spans="4:4" ht="15.75" customHeight="1">
+    <row r="377" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D377" s="3"/>
     </row>
-    <row r="378" spans="4:4" ht="15.75" customHeight="1">
+    <row r="378" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D378" s="3"/>
     </row>
-    <row r="379" spans="4:4" ht="15.75" customHeight="1">
+    <row r="379" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D379" s="3"/>
     </row>
-    <row r="380" spans="4:4" ht="15.75" customHeight="1">
+    <row r="380" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D380" s="3"/>
     </row>
-    <row r="381" spans="4:4" ht="15.75" customHeight="1">
+    <row r="381" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D381" s="3"/>
     </row>
-    <row r="382" spans="4:4" ht="15.75" customHeight="1">
+    <row r="382" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D382" s="3"/>
     </row>
-    <row r="383" spans="4:4" ht="15.75" customHeight="1">
+    <row r="383" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D383" s="3"/>
     </row>
-    <row r="384" spans="4:4" ht="15.75" customHeight="1">
+    <row r="384" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D384" s="3"/>
     </row>
-    <row r="385" spans="4:4" ht="15.75" customHeight="1">
+    <row r="385" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D385" s="3"/>
     </row>
-    <row r="386" spans="4:4" ht="15.75" customHeight="1">
+    <row r="386" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D386" s="3"/>
     </row>
-    <row r="387" spans="4:4" ht="15.75" customHeight="1">
+    <row r="387" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D387" s="3"/>
     </row>
-    <row r="388" spans="4:4" ht="15.75" customHeight="1">
+    <row r="388" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D388" s="3"/>
     </row>
-    <row r="389" spans="4:4" ht="15.75" customHeight="1">
+    <row r="389" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D389" s="3"/>
     </row>
-    <row r="390" spans="4:4" ht="15.75" customHeight="1">
+    <row r="390" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D390" s="3"/>
     </row>
-    <row r="391" spans="4:4" ht="15.75" customHeight="1">
+    <row r="391" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D391" s="3"/>
     </row>
-    <row r="392" spans="4:4" ht="15.75" customHeight="1">
+    <row r="392" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D392" s="3"/>
     </row>
-    <row r="393" spans="4:4" ht="15.75" customHeight="1">
+    <row r="393" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D393" s="3"/>
     </row>
-    <row r="394" spans="4:4" ht="15.75" customHeight="1">
+    <row r="394" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D394" s="3"/>
     </row>
-    <row r="395" spans="4:4" ht="15.75" customHeight="1">
+    <row r="395" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D395" s="3"/>
     </row>
-    <row r="396" spans="4:4" ht="15.75" customHeight="1">
+    <row r="396" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D396" s="3"/>
     </row>
-    <row r="397" spans="4:4" ht="15.75" customHeight="1">
+    <row r="397" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D397" s="3"/>
     </row>
-    <row r="398" spans="4:4" ht="15.75" customHeight="1">
+    <row r="398" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D398" s="3"/>
     </row>
-    <row r="399" spans="4:4" ht="15.75" customHeight="1">
+    <row r="399" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D399" s="3"/>
     </row>
-    <row r="400" spans="4:4" ht="15.75" customHeight="1">
+    <row r="400" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D400" s="3"/>
     </row>
-    <row r="401" spans="4:4" ht="15.75" customHeight="1">
+    <row r="401" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D401" s="3"/>
     </row>
-    <row r="402" spans="4:4" ht="15.75" customHeight="1">
+    <row r="402" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D402" s="3"/>
     </row>
-    <row r="403" spans="4:4" ht="15.75" customHeight="1">
+    <row r="403" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D403" s="3"/>
     </row>
-    <row r="404" spans="4:4" ht="15.75" customHeight="1">
+    <row r="404" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D404" s="3"/>
     </row>
-    <row r="405" spans="4:4" ht="15.75" customHeight="1">
+    <row r="405" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D405" s="3"/>
     </row>
-    <row r="406" spans="4:4" ht="15.75" customHeight="1">
+    <row r="406" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D406" s="3"/>
     </row>
-    <row r="407" spans="4:4" ht="15.75" customHeight="1">
+    <row r="407" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D407" s="3"/>
     </row>
-    <row r="408" spans="4:4" ht="15.75" customHeight="1">
+    <row r="408" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D408" s="3"/>
     </row>
-    <row r="409" spans="4:4" ht="15.75" customHeight="1">
+    <row r="409" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D409" s="3"/>
     </row>
-    <row r="410" spans="4:4" ht="15.75" customHeight="1">
+    <row r="410" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D410" s="3"/>
     </row>
-    <row r="411" spans="4:4" ht="15.75" customHeight="1">
+    <row r="411" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D411" s="3"/>
     </row>
-    <row r="412" spans="4:4" ht="15.75" customHeight="1">
+    <row r="412" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D412" s="3"/>
     </row>
-    <row r="413" spans="4:4" ht="15.75" customHeight="1">
+    <row r="413" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D413" s="3"/>
     </row>
-    <row r="414" spans="4:4" ht="15.75" customHeight="1">
+    <row r="414" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D414" s="3"/>
     </row>
-    <row r="415" spans="4:4" ht="15.75" customHeight="1">
+    <row r="415" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D415" s="3"/>
     </row>
-    <row r="416" spans="4:4" ht="15.75" customHeight="1">
+    <row r="416" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D416" s="3"/>
     </row>
-    <row r="417" spans="4:4" ht="15.75" customHeight="1">
+    <row r="417" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D417" s="3"/>
     </row>
-    <row r="418" spans="4:4" ht="15.75" customHeight="1">
+    <row r="418" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D418" s="3"/>
     </row>
-    <row r="419" spans="4:4" ht="15.75" customHeight="1">
+    <row r="419" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D419" s="3"/>
     </row>
-    <row r="420" spans="4:4" ht="15.75" customHeight="1">
+    <row r="420" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D420" s="3"/>
     </row>
-    <row r="421" spans="4:4" ht="15.75" customHeight="1">
+    <row r="421" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D421" s="3"/>
     </row>
-    <row r="422" spans="4:4" ht="15.75" customHeight="1">
+    <row r="422" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D422" s="3"/>
     </row>
-    <row r="423" spans="4:4" ht="15.75" customHeight="1">
+    <row r="423" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D423" s="3"/>
     </row>
-    <row r="424" spans="4:4" ht="15.75" customHeight="1">
+    <row r="424" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D424" s="3"/>
     </row>
-    <row r="425" spans="4:4" ht="15.75" customHeight="1">
+    <row r="425" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D425" s="3"/>
     </row>
-    <row r="426" spans="4:4" ht="15.75" customHeight="1">
+    <row r="426" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D426" s="3"/>
     </row>
-    <row r="427" spans="4:4" ht="15.75" customHeight="1">
+    <row r="427" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D427" s="3"/>
     </row>
-    <row r="428" spans="4:4" ht="15.75" customHeight="1">
+    <row r="428" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D428" s="3"/>
     </row>
-    <row r="429" spans="4:4" ht="15.75" customHeight="1">
+    <row r="429" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D429" s="3"/>
     </row>
-    <row r="430" spans="4:4" ht="15.75" customHeight="1">
+    <row r="430" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D430" s="3"/>
     </row>
-    <row r="431" spans="4:4" ht="15.75" customHeight="1">
+    <row r="431" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D431" s="3"/>
     </row>
-    <row r="432" spans="4:4" ht="15.75" customHeight="1">
+    <row r="432" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D432" s="3"/>
     </row>
-    <row r="433" spans="4:4" ht="15.75" customHeight="1">
+    <row r="433" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D433" s="3"/>
     </row>
-    <row r="434" spans="4:4" ht="15.75" customHeight="1">
+    <row r="434" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D434" s="3"/>
     </row>
-    <row r="435" spans="4:4" ht="15.75" customHeight="1">
+    <row r="435" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D435" s="3"/>
     </row>
-    <row r="436" spans="4:4" ht="15.75" customHeight="1">
+    <row r="436" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D436" s="3"/>
     </row>
-    <row r="437" spans="4:4" ht="15.75" customHeight="1">
+    <row r="437" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D437" s="3"/>
     </row>
-    <row r="438" spans="4:4" ht="15.75" customHeight="1">
+    <row r="438" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D438" s="3"/>
     </row>
-    <row r="439" spans="4:4" ht="15.75" customHeight="1">
+    <row r="439" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D439" s="3"/>
     </row>
-    <row r="440" spans="4:4" ht="15.75" customHeight="1">
+    <row r="440" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D440" s="3"/>
     </row>
-    <row r="441" spans="4:4" ht="15.75" customHeight="1">
+    <row r="441" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D441" s="3"/>
     </row>
-    <row r="442" spans="4:4" ht="15.75" customHeight="1">
+    <row r="442" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D442" s="3"/>
     </row>
-    <row r="443" spans="4:4" ht="15.75" customHeight="1">
+    <row r="443" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D443" s="3"/>
     </row>
-    <row r="444" spans="4:4" ht="15.75" customHeight="1">
+    <row r="444" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D444" s="3"/>
     </row>
-    <row r="445" spans="4:4" ht="15.75" customHeight="1">
+    <row r="445" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D445" s="3"/>
     </row>
-    <row r="446" spans="4:4" ht="15.75" customHeight="1">
+    <row r="446" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D446" s="3"/>
     </row>
-    <row r="447" spans="4:4" ht="15.75" customHeight="1">
+    <row r="447" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D447" s="3"/>
     </row>
-    <row r="448" spans="4:4" ht="15.75" customHeight="1">
+    <row r="448" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D448" s="3"/>
     </row>
-    <row r="449" spans="4:4" ht="15.75" customHeight="1">
+    <row r="449" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D449" s="3"/>
     </row>
-    <row r="450" spans="4:4" ht="15.75" customHeight="1">
+    <row r="450" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D450" s="3"/>
     </row>
-    <row r="451" spans="4:4" ht="15.75" customHeight="1">
+    <row r="451" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D451" s="3"/>
     </row>
-    <row r="452" spans="4:4" ht="15.75" customHeight="1">
+    <row r="452" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D452" s="3"/>
     </row>
-    <row r="453" spans="4:4" ht="15.75" customHeight="1">
+    <row r="453" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D453" s="3"/>
     </row>
-    <row r="454" spans="4:4" ht="15.75" customHeight="1">
+    <row r="454" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D454" s="3"/>
     </row>
-    <row r="455" spans="4:4" ht="15.75" customHeight="1">
+    <row r="455" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D455" s="3"/>
     </row>
-    <row r="456" spans="4:4" ht="15.75" customHeight="1">
+    <row r="456" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D456" s="3"/>
     </row>
-    <row r="457" spans="4:4" ht="15.75" customHeight="1">
+    <row r="457" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D457" s="3"/>
     </row>
-    <row r="458" spans="4:4" ht="15.75" customHeight="1">
+    <row r="458" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D458" s="3"/>
     </row>
-    <row r="459" spans="4:4" ht="15.75" customHeight="1">
+    <row r="459" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D459" s="3"/>
     </row>
-    <row r="460" spans="4:4" ht="15.75" customHeight="1">
+    <row r="460" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D460" s="3"/>
     </row>
-    <row r="461" spans="4:4" ht="15.75" customHeight="1">
+    <row r="461" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D461" s="3"/>
     </row>
-    <row r="462" spans="4:4" ht="15.75" customHeight="1">
+    <row r="462" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D462" s="3"/>
     </row>
-    <row r="463" spans="4:4" ht="15.75" customHeight="1">
+    <row r="463" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D463" s="3"/>
     </row>
-    <row r="464" spans="4:4" ht="15.75" customHeight="1">
+    <row r="464" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D464" s="3"/>
     </row>
-    <row r="465" spans="4:4" ht="15.75" customHeight="1">
+    <row r="465" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D465" s="3"/>
     </row>
-    <row r="466" spans="4:4" ht="15.75" customHeight="1">
+    <row r="466" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D466" s="3"/>
     </row>
-    <row r="467" spans="4:4" ht="15.75" customHeight="1">
+    <row r="467" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D467" s="3"/>
     </row>
-    <row r="468" spans="4:4" ht="15.75" customHeight="1">
+    <row r="468" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D468" s="3"/>
     </row>
-    <row r="469" spans="4:4" ht="15.75" customHeight="1">
+    <row r="469" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D469" s="3"/>
     </row>
-    <row r="470" spans="4:4" ht="15.75" customHeight="1">
+    <row r="470" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D470" s="3"/>
     </row>
-    <row r="471" spans="4:4" ht="15.75" customHeight="1">
+    <row r="471" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D471" s="3"/>
     </row>
-    <row r="472" spans="4:4" ht="15.75" customHeight="1">
+    <row r="472" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D472" s="3"/>
     </row>
-    <row r="473" spans="4:4" ht="15.75" customHeight="1">
+    <row r="473" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D473" s="3"/>
     </row>
-    <row r="474" spans="4:4" ht="15.75" customHeight="1">
+    <row r="474" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D474" s="3"/>
     </row>
-    <row r="475" spans="4:4" ht="15.75" customHeight="1">
+    <row r="475" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D475" s="3"/>
     </row>
-    <row r="476" spans="4:4" ht="15.75" customHeight="1">
+    <row r="476" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D476" s="3"/>
     </row>
-    <row r="477" spans="4:4" ht="15.75" customHeight="1">
+    <row r="477" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D477" s="3"/>
     </row>
-    <row r="478" spans="4:4" ht="15.75" customHeight="1">
+    <row r="478" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D478" s="3"/>
     </row>
-    <row r="479" spans="4:4" ht="15.75" customHeight="1">
+    <row r="479" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D479" s="3"/>
     </row>
-    <row r="480" spans="4:4" ht="15.75" customHeight="1">
+    <row r="480" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D480" s="3"/>
     </row>
-    <row r="481" spans="4:4" ht="15.75" customHeight="1">
+    <row r="481" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D481" s="3"/>
     </row>
-    <row r="482" spans="4:4" ht="15.75" customHeight="1">
+    <row r="482" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D482" s="3"/>
     </row>
-    <row r="483" spans="4:4" ht="15.75" customHeight="1">
+    <row r="483" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D483" s="3"/>
     </row>
-    <row r="484" spans="4:4" ht="15.75" customHeight="1">
+    <row r="484" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D484" s="3"/>
     </row>
-    <row r="485" spans="4:4" ht="15.75" customHeight="1">
+    <row r="485" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D485" s="3"/>
     </row>
-    <row r="486" spans="4:4" ht="15.75" customHeight="1">
+    <row r="486" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D486" s="3"/>
     </row>
-    <row r="487" spans="4:4" ht="15.75" customHeight="1">
+    <row r="487" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D487" s="3"/>
     </row>
-    <row r="488" spans="4:4" ht="15.75" customHeight="1">
+    <row r="488" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D488" s="3"/>
     </row>
-    <row r="489" spans="4:4" ht="15.75" customHeight="1">
+    <row r="489" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D489" s="3"/>
     </row>
-    <row r="490" spans="4:4" ht="15.75" customHeight="1">
+    <row r="490" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D490" s="3"/>
     </row>
-    <row r="491" spans="4:4" ht="15.75" customHeight="1">
+    <row r="491" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D491" s="3"/>
     </row>
-    <row r="492" spans="4:4" ht="15.75" customHeight="1">
+    <row r="492" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D492" s="3"/>
     </row>
-    <row r="493" spans="4:4" ht="15.75" customHeight="1">
+    <row r="493" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D493" s="3"/>
     </row>
-    <row r="494" spans="4:4" ht="15.75" customHeight="1">
+    <row r="494" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D494" s="3"/>
     </row>
-    <row r="495" spans="4:4" ht="15.75" customHeight="1">
+    <row r="495" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D495" s="3"/>
     </row>
-    <row r="496" spans="4:4" ht="15.75" customHeight="1">
+    <row r="496" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D496" s="3"/>
     </row>
-    <row r="497" spans="4:4" ht="15.75" customHeight="1">
+    <row r="497" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D497" s="3"/>
     </row>
-    <row r="498" spans="4:4" ht="15.75" customHeight="1">
+    <row r="498" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D498" s="3"/>
     </row>
-    <row r="499" spans="4:4" ht="15.75" customHeight="1">
+    <row r="499" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D499" s="3"/>
     </row>
-    <row r="500" spans="4:4" ht="15.75" customHeight="1">
+    <row r="500" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D500" s="3"/>
     </row>
-    <row r="501" spans="4:4" ht="15.75" customHeight="1">
+    <row r="501" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D501" s="3"/>
     </row>
-    <row r="502" spans="4:4" ht="15.75" customHeight="1">
+    <row r="502" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D502" s="3"/>
     </row>
-    <row r="503" spans="4:4" ht="15.75" customHeight="1">
+    <row r="503" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D503" s="3"/>
     </row>
-    <row r="504" spans="4:4" ht="15.75" customHeight="1">
+    <row r="504" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D504" s="3"/>
     </row>
-    <row r="505" spans="4:4" ht="15.75" customHeight="1">
+    <row r="505" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D505" s="3"/>
     </row>
-    <row r="506" spans="4:4" ht="15.75" customHeight="1">
+    <row r="506" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D506" s="3"/>
     </row>
-    <row r="507" spans="4:4" ht="15.75" customHeight="1">
+    <row r="507" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D507" s="3"/>
     </row>
-    <row r="508" spans="4:4" ht="15.75" customHeight="1">
+    <row r="508" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D508" s="3"/>
     </row>
-    <row r="509" spans="4:4" ht="15.75" customHeight="1">
+    <row r="509" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D509" s="3"/>
     </row>
-    <row r="510" spans="4:4" ht="15.75" customHeight="1">
+    <row r="510" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D510" s="3"/>
     </row>
-    <row r="511" spans="4:4" ht="15.75" customHeight="1">
+    <row r="511" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D511" s="3"/>
     </row>
-    <row r="512" spans="4:4" ht="15.75" customHeight="1">
+    <row r="512" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D512" s="3"/>
     </row>
-    <row r="513" spans="4:4" ht="15.75" customHeight="1">
+    <row r="513" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D513" s="3"/>
     </row>
-    <row r="514" spans="4:4" ht="15.75" customHeight="1">
+    <row r="514" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D514" s="3"/>
     </row>
-    <row r="515" spans="4:4" ht="15.75" customHeight="1">
+    <row r="515" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D515" s="3"/>
     </row>
-    <row r="516" spans="4:4" ht="15.75" customHeight="1">
+    <row r="516" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D516" s="3"/>
     </row>
-    <row r="517" spans="4:4" ht="15.75" customHeight="1">
+    <row r="517" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D517" s="3"/>
     </row>
-    <row r="518" spans="4:4" ht="15.75" customHeight="1">
+    <row r="518" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D518" s="3"/>
     </row>
-    <row r="519" spans="4:4" ht="15.75" customHeight="1">
+    <row r="519" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D519" s="3"/>
     </row>
-    <row r="520" spans="4:4" ht="15.75" customHeight="1">
+    <row r="520" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D520" s="3"/>
     </row>
-    <row r="521" spans="4:4" ht="15.75" customHeight="1">
+    <row r="521" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D521" s="3"/>
     </row>
-    <row r="522" spans="4:4" ht="15.75" customHeight="1">
+    <row r="522" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D522" s="3"/>
     </row>
-    <row r="523" spans="4:4" ht="15.75" customHeight="1">
+    <row r="523" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D523" s="3"/>
     </row>
-    <row r="524" spans="4:4" ht="15.75" customHeight="1">
+    <row r="524" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D524" s="3"/>
     </row>
-    <row r="525" spans="4:4" ht="15.75" customHeight="1">
+    <row r="525" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D525" s="3"/>
     </row>
-    <row r="526" spans="4:4" ht="15.75" customHeight="1">
+    <row r="526" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D526" s="3"/>
     </row>
-    <row r="527" spans="4:4" ht="15.75" customHeight="1">
+    <row r="527" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D527" s="3"/>
     </row>
-    <row r="528" spans="4:4" ht="15.75" customHeight="1">
+    <row r="528" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D528" s="3"/>
     </row>
-    <row r="529" spans="4:4" ht="15.75" customHeight="1">
+    <row r="529" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D529" s="3"/>
     </row>
-    <row r="530" spans="4:4" ht="15.75" customHeight="1">
+    <row r="530" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D530" s="3"/>
     </row>
-    <row r="531" spans="4:4" ht="15.75" customHeight="1">
+    <row r="531" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D531" s="3"/>
     </row>
-    <row r="532" spans="4:4" ht="15.75" customHeight="1">
+    <row r="532" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D532" s="3"/>
     </row>
-    <row r="533" spans="4:4" ht="15.75" customHeight="1">
+    <row r="533" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D533" s="3"/>
     </row>
-    <row r="534" spans="4:4" ht="15.75" customHeight="1">
+    <row r="534" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D534" s="3"/>
     </row>
-    <row r="535" spans="4:4" ht="15.75" customHeight="1">
+    <row r="535" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D535" s="3"/>
     </row>
-    <row r="536" spans="4:4" ht="15.75" customHeight="1">
+    <row r="536" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D536" s="3"/>
     </row>
-    <row r="537" spans="4:4" ht="15.75" customHeight="1">
+    <row r="537" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D537" s="3"/>
     </row>
-    <row r="538" spans="4:4" ht="15.75" customHeight="1">
+    <row r="538" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D538" s="3"/>
     </row>
-    <row r="539" spans="4:4" ht="15.75" customHeight="1">
+    <row r="539" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D539" s="3"/>
     </row>
-    <row r="540" spans="4:4" ht="15.75" customHeight="1">
+    <row r="540" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D540" s="3"/>
     </row>
-    <row r="541" spans="4:4" ht="15.75" customHeight="1">
+    <row r="541" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D541" s="3"/>
     </row>
-    <row r="542" spans="4:4" ht="15.75" customHeight="1">
+    <row r="542" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D542" s="3"/>
     </row>
-    <row r="543" spans="4:4" ht="15.75" customHeight="1">
+    <row r="543" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D543" s="3"/>
     </row>
-    <row r="544" spans="4:4" ht="15.75" customHeight="1">
+    <row r="544" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D544" s="3"/>
     </row>
-    <row r="545" spans="4:4" ht="15.75" customHeight="1">
+    <row r="545" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D545" s="3"/>
     </row>
-    <row r="546" spans="4:4" ht="15.75" customHeight="1">
+    <row r="546" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D546" s="3"/>
     </row>
-    <row r="547" spans="4:4" ht="15.75" customHeight="1">
+    <row r="547" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D547" s="3"/>
     </row>
-    <row r="548" spans="4:4" ht="15.75" customHeight="1">
+    <row r="548" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D548" s="3"/>
     </row>
-    <row r="549" spans="4:4" ht="15.75" customHeight="1">
+    <row r="549" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D549" s="3"/>
     </row>
-    <row r="550" spans="4:4" ht="15.75" customHeight="1">
+    <row r="550" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D550" s="3"/>
     </row>
-    <row r="551" spans="4:4" ht="15.75" customHeight="1">
+    <row r="551" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D551" s="3"/>
     </row>
-    <row r="552" spans="4:4" ht="15.75" customHeight="1">
+    <row r="552" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D552" s="3"/>
     </row>
-    <row r="553" spans="4:4" ht="15.75" customHeight="1">
+    <row r="553" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D553" s="3"/>
     </row>
-    <row r="554" spans="4:4" ht="15.75" customHeight="1">
+    <row r="554" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D554" s="3"/>
     </row>
-    <row r="555" spans="4:4" ht="15.75" customHeight="1">
+    <row r="555" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D555" s="3"/>
     </row>
-    <row r="556" spans="4:4" ht="15.75" customHeight="1">
+    <row r="556" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D556" s="3"/>
     </row>
-    <row r="557" spans="4:4" ht="15.75" customHeight="1">
+    <row r="557" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D557" s="3"/>
     </row>
-    <row r="558" spans="4:4" ht="15.75" customHeight="1">
+    <row r="558" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D558" s="3"/>
     </row>
-    <row r="559" spans="4:4" ht="15.75" customHeight="1">
+    <row r="559" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D559" s="3"/>
     </row>
-    <row r="560" spans="4:4" ht="15.75" customHeight="1">
+    <row r="560" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D560" s="3"/>
     </row>
-    <row r="561" spans="4:4" ht="15.75" customHeight="1">
+    <row r="561" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D561" s="3"/>
     </row>
-    <row r="562" spans="4:4" ht="15.75" customHeight="1">
+    <row r="562" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D562" s="3"/>
     </row>
-    <row r="563" spans="4:4" ht="15.75" customHeight="1">
+    <row r="563" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D563" s="3"/>
     </row>
-    <row r="564" spans="4:4" ht="15.75" customHeight="1">
+    <row r="564" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D564" s="3"/>
     </row>
-    <row r="565" spans="4:4" ht="15.75" customHeight="1">
+    <row r="565" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D565" s="3"/>
     </row>
-    <row r="566" spans="4:4" ht="15.75" customHeight="1">
+    <row r="566" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D566" s="3"/>
     </row>
-    <row r="567" spans="4:4" ht="15.75" customHeight="1">
+    <row r="567" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D567" s="3"/>
     </row>
-    <row r="568" spans="4:4" ht="15.75" customHeight="1">
+    <row r="568" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D568" s="3"/>
     </row>
-    <row r="569" spans="4:4" ht="15.75" customHeight="1">
+    <row r="569" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D569" s="3"/>
     </row>
-    <row r="570" spans="4:4" ht="15.75" customHeight="1">
+    <row r="570" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D570" s="3"/>
     </row>
-    <row r="571" spans="4:4" ht="15.75" customHeight="1">
+    <row r="571" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D571" s="3"/>
     </row>
-    <row r="572" spans="4:4" ht="15.75" customHeight="1">
+    <row r="572" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D572" s="3"/>
     </row>
-    <row r="573" spans="4:4" ht="15.75" customHeight="1">
+    <row r="573" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D573" s="3"/>
     </row>
-    <row r="574" spans="4:4" ht="15.75" customHeight="1">
+    <row r="574" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D574" s="3"/>
     </row>
-    <row r="575" spans="4:4" ht="15.75" customHeight="1">
+    <row r="575" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D575" s="3"/>
     </row>
-    <row r="576" spans="4:4" ht="15.75" customHeight="1">
+    <row r="576" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D576" s="3"/>
     </row>
-    <row r="577" spans="4:4" ht="15.75" customHeight="1">
+    <row r="577" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D577" s="3"/>
     </row>
-    <row r="578" spans="4:4" ht="15.75" customHeight="1">
+    <row r="578" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D578" s="3"/>
     </row>
-    <row r="579" spans="4:4" ht="15.75" customHeight="1">
+    <row r="579" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D579" s="3"/>
     </row>
-    <row r="580" spans="4:4" ht="15.75" customHeight="1">
+    <row r="580" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D580" s="3"/>
     </row>
-    <row r="581" spans="4:4" ht="15.75" customHeight="1">
+    <row r="581" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D581" s="3"/>
     </row>
-    <row r="582" spans="4:4" ht="15.75" customHeight="1">
+    <row r="582" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D582" s="3"/>
     </row>
-    <row r="583" spans="4:4" ht="15.75" customHeight="1">
+    <row r="583" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D583" s="3"/>
     </row>
-    <row r="584" spans="4:4" ht="15.75" customHeight="1">
+    <row r="584" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D584" s="3"/>
     </row>
-    <row r="585" spans="4:4" ht="15.75" customHeight="1">
+    <row r="585" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D585" s="3"/>
     </row>
-    <row r="586" spans="4:4" ht="15.75" customHeight="1">
+    <row r="586" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D586" s="3"/>
     </row>
-    <row r="587" spans="4:4" ht="15.75" customHeight="1">
+    <row r="587" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D587" s="3"/>
     </row>
-    <row r="588" spans="4:4" ht="15.75" customHeight="1">
+    <row r="588" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D588" s="3"/>
     </row>
-    <row r="589" spans="4:4" ht="15.75" customHeight="1">
+    <row r="589" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D589" s="3"/>
     </row>
-    <row r="590" spans="4:4" ht="15.75" customHeight="1">
+    <row r="590" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D590" s="3"/>
     </row>
-    <row r="591" spans="4:4" ht="15.75" customHeight="1">
+    <row r="591" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D591" s="3"/>
     </row>
-    <row r="592" spans="4:4" ht="15.75" customHeight="1">
+    <row r="592" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D592" s="3"/>
     </row>
-    <row r="593" spans="4:4" ht="15.75" customHeight="1">
+    <row r="593" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D593" s="3"/>
     </row>
-    <row r="594" spans="4:4" ht="15.75" customHeight="1">
+    <row r="594" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D594" s="3"/>
     </row>
-    <row r="595" spans="4:4" ht="15.75" customHeight="1">
+    <row r="595" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D595" s="3"/>
     </row>
-    <row r="596" spans="4:4" ht="15.75" customHeight="1">
+    <row r="596" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D596" s="3"/>
     </row>
-    <row r="597" spans="4:4" ht="15.75" customHeight="1">
+    <row r="597" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D597" s="3"/>
     </row>
-    <row r="598" spans="4:4" ht="15.75" customHeight="1">
+    <row r="598" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D598" s="3"/>
     </row>
-    <row r="599" spans="4:4" ht="15.75" customHeight="1">
+    <row r="599" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D599" s="3"/>
     </row>
-    <row r="600" spans="4:4" ht="15.75" customHeight="1">
+    <row r="600" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D600" s="3"/>
     </row>
-    <row r="601" spans="4:4" ht="15.75" customHeight="1">
+    <row r="601" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D601" s="3"/>
     </row>
-    <row r="602" spans="4:4" ht="15.75" customHeight="1">
+    <row r="602" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D602" s="3"/>
     </row>
-    <row r="603" spans="4:4" ht="15.75" customHeight="1">
+    <row r="603" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D603" s="3"/>
     </row>
-    <row r="604" spans="4:4" ht="15.75" customHeight="1">
+    <row r="604" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D604" s="3"/>
     </row>
-    <row r="605" spans="4:4" ht="15.75" customHeight="1">
+    <row r="605" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D605" s="3"/>
     </row>
-    <row r="606" spans="4:4" ht="15.75" customHeight="1">
+    <row r="606" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D606" s="3"/>
     </row>
-    <row r="607" spans="4:4" ht="15.75" customHeight="1">
+    <row r="607" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D607" s="3"/>
     </row>
-    <row r="608" spans="4:4" ht="15.75" customHeight="1">
+    <row r="608" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D608" s="3"/>
     </row>
-    <row r="609" spans="4:4" ht="15.75" customHeight="1">
+    <row r="609" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D609" s="3"/>
     </row>
-    <row r="610" spans="4:4" ht="15.75" customHeight="1">
+    <row r="610" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D610" s="3"/>
     </row>
-    <row r="611" spans="4:4" ht="15.75" customHeight="1">
+    <row r="611" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D611" s="3"/>
     </row>
-    <row r="612" spans="4:4" ht="15.75" customHeight="1">
+    <row r="612" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D612" s="3"/>
     </row>
-    <row r="613" spans="4:4" ht="15.75" customHeight="1">
+    <row r="613" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D613" s="3"/>
     </row>
-    <row r="614" spans="4:4" ht="15.75" customHeight="1">
+    <row r="614" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D614" s="3"/>
     </row>
-    <row r="615" spans="4:4" ht="15.75" customHeight="1">
+    <row r="615" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D615" s="3"/>
     </row>
-    <row r="616" spans="4:4" ht="15.75" customHeight="1">
+    <row r="616" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D616" s="3"/>
     </row>
-    <row r="617" spans="4:4" ht="15.75" customHeight="1">
+    <row r="617" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D617" s="3"/>
     </row>
-    <row r="618" spans="4:4" ht="15.75" customHeight="1">
+    <row r="618" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D618" s="3"/>
     </row>
-    <row r="619" spans="4:4" ht="15.75" customHeight="1">
+    <row r="619" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D619" s="3"/>
     </row>
-    <row r="620" spans="4:4" ht="15.75" customHeight="1">
+    <row r="620" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D620" s="3"/>
     </row>
-    <row r="621" spans="4:4" ht="15.75" customHeight="1">
+    <row r="621" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D621" s="3"/>
     </row>
-    <row r="622" spans="4:4" ht="15.75" customHeight="1">
+    <row r="622" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D622" s="3"/>
     </row>
-    <row r="623" spans="4:4" ht="15.75" customHeight="1">
+    <row r="623" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D623" s="3"/>
     </row>
-    <row r="624" spans="4:4" ht="15.75" customHeight="1">
+    <row r="624" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D624" s="3"/>
     </row>
-    <row r="625" spans="4:4" ht="15.75" customHeight="1">
+    <row r="625" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D625" s="3"/>
     </row>
-    <row r="626" spans="4:4" ht="15.75" customHeight="1">
+    <row r="626" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D626" s="3"/>
     </row>
-    <row r="627" spans="4:4" ht="15.75" customHeight="1">
+    <row r="627" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D627" s="3"/>
     </row>
-    <row r="628" spans="4:4" ht="15.75" customHeight="1">
+    <row r="628" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D628" s="3"/>
     </row>
-    <row r="629" spans="4:4" ht="15.75" customHeight="1">
+    <row r="629" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D629" s="3"/>
     </row>
-    <row r="630" spans="4:4" ht="15.75" customHeight="1">
+    <row r="630" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D630" s="3"/>
     </row>
-    <row r="631" spans="4:4" ht="15.75" customHeight="1">
+    <row r="631" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D631" s="3"/>
     </row>
-    <row r="632" spans="4:4" ht="15.75" customHeight="1">
+    <row r="632" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D632" s="3"/>
     </row>
-    <row r="633" spans="4:4" ht="15.75" customHeight="1">
+    <row r="633" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D633" s="3"/>
     </row>
-    <row r="634" spans="4:4" ht="15.75" customHeight="1">
+    <row r="634" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D634" s="3"/>
     </row>
-    <row r="635" spans="4:4" ht="15.75" customHeight="1">
+    <row r="635" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D635" s="3"/>
     </row>
-    <row r="636" spans="4:4" ht="15.75" customHeight="1">
+    <row r="636" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D636" s="3"/>
     </row>
-    <row r="637" spans="4:4" ht="15.75" customHeight="1">
+    <row r="637" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D637" s="3"/>
     </row>
-    <row r="638" spans="4:4" ht="15.75" customHeight="1">
+    <row r="638" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D638" s="3"/>
     </row>
-    <row r="639" spans="4:4" ht="15.75" customHeight="1">
+    <row r="639" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D639" s="3"/>
     </row>
-    <row r="640" spans="4:4" ht="15.75" customHeight="1">
+    <row r="640" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D640" s="3"/>
     </row>
-    <row r="641" spans="4:4" ht="15.75" customHeight="1">
+    <row r="641" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D641" s="3"/>
     </row>
-    <row r="642" spans="4:4" ht="15.75" customHeight="1">
+    <row r="642" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D642" s="3"/>
     </row>
-    <row r="643" spans="4:4" ht="15.75" customHeight="1">
+    <row r="643" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D643" s="3"/>
     </row>
-    <row r="644" spans="4:4" ht="15.75" customHeight="1">
+    <row r="644" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D644" s="3"/>
     </row>
-    <row r="645" spans="4:4" ht="15.75" customHeight="1">
+    <row r="645" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D645" s="3"/>
     </row>
-    <row r="646" spans="4:4" ht="15.75" customHeight="1">
+    <row r="646" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D646" s="3"/>
     </row>
-    <row r="647" spans="4:4" ht="15.75" customHeight="1">
+    <row r="647" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D647" s="3"/>
     </row>
-    <row r="648" spans="4:4" ht="15.75" customHeight="1">
+    <row r="648" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D648" s="3"/>
     </row>
-    <row r="649" spans="4:4" ht="15.75" customHeight="1">
+    <row r="649" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D649" s="3"/>
     </row>
-    <row r="650" spans="4:4" ht="15.75" customHeight="1">
+    <row r="650" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D650" s="3"/>
     </row>
-    <row r="651" spans="4:4" ht="15.75" customHeight="1">
+    <row r="651" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D651" s="3"/>
     </row>
-    <row r="652" spans="4:4" ht="15.75" customHeight="1">
+    <row r="652" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D652" s="3"/>
     </row>
-    <row r="653" spans="4:4" ht="15.75" customHeight="1">
+    <row r="653" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D653" s="3"/>
     </row>
-    <row r="654" spans="4:4" ht="15.75" customHeight="1">
+    <row r="654" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D654" s="3"/>
     </row>
-    <row r="655" spans="4:4" ht="15.75" customHeight="1">
+    <row r="655" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D655" s="3"/>
     </row>
-    <row r="656" spans="4:4" ht="15.75" customHeight="1">
+    <row r="656" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D656" s="3"/>
     </row>
-    <row r="657" spans="4:4" ht="15.75" customHeight="1">
+    <row r="657" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D657" s="3"/>
     </row>
-    <row r="658" spans="4:4" ht="15.75" customHeight="1">
+    <row r="658" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D658" s="3"/>
     </row>
-    <row r="659" spans="4:4" ht="15.75" customHeight="1">
+    <row r="659" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D659" s="3"/>
     </row>
-    <row r="660" spans="4:4" ht="15.75" customHeight="1">
+    <row r="660" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D660" s="3"/>
     </row>
-    <row r="661" spans="4:4" ht="15.75" customHeight="1">
+    <row r="661" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D661" s="3"/>
     </row>
-    <row r="662" spans="4:4" ht="15.75" customHeight="1">
+    <row r="662" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D662" s="3"/>
     </row>
-    <row r="663" spans="4:4" ht="15.75" customHeight="1">
+    <row r="663" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D663" s="3"/>
     </row>
-    <row r="664" spans="4:4" ht="15.75" customHeight="1">
+    <row r="664" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D664" s="3"/>
     </row>
-    <row r="665" spans="4:4" ht="15.75" customHeight="1">
+    <row r="665" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D665" s="3"/>
     </row>
-    <row r="666" spans="4:4" ht="15.75" customHeight="1">
+    <row r="666" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D666" s="3"/>
     </row>
-    <row r="667" spans="4:4" ht="15.75" customHeight="1">
+    <row r="667" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D667" s="3"/>
     </row>
-    <row r="668" spans="4:4" ht="15.75" customHeight="1">
+    <row r="668" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D668" s="3"/>
     </row>
-    <row r="669" spans="4:4" ht="15.75" customHeight="1">
+    <row r="669" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D669" s="3"/>
     </row>
-    <row r="670" spans="4:4" ht="15.75" customHeight="1">
+    <row r="670" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D670" s="3"/>
     </row>
-    <row r="671" spans="4:4" ht="15.75" customHeight="1">
+    <row r="671" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D671" s="3"/>
     </row>
-    <row r="672" spans="4:4" ht="15.75" customHeight="1">
+    <row r="672" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D672" s="3"/>
     </row>
-    <row r="673" spans="4:4" ht="15.75" customHeight="1">
+    <row r="673" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D673" s="3"/>
     </row>
-    <row r="674" spans="4:4" ht="15.75" customHeight="1">
+    <row r="674" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D674" s="3"/>
     </row>
-    <row r="675" spans="4:4" ht="15.75" customHeight="1">
+    <row r="675" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D675" s="3"/>
     </row>
-    <row r="676" spans="4:4" ht="15.75" customHeight="1">
+    <row r="676" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D676" s="3"/>
     </row>
-    <row r="677" spans="4:4" ht="15.75" customHeight="1">
+    <row r="677" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D677" s="3"/>
     </row>
-    <row r="678" spans="4:4" ht="15.75" customHeight="1">
+    <row r="678" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D678" s="3"/>
     </row>
-    <row r="679" spans="4:4" ht="15.75" customHeight="1">
+    <row r="679" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D679" s="3"/>
     </row>
-    <row r="680" spans="4:4" ht="15.75" customHeight="1">
+    <row r="680" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D680" s="3"/>
     </row>
-    <row r="681" spans="4:4" ht="15.75" customHeight="1">
+    <row r="681" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D681" s="3"/>
     </row>
-    <row r="682" spans="4:4" ht="15.75" customHeight="1">
+    <row r="682" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D682" s="3"/>
     </row>
-    <row r="683" spans="4:4" ht="15.75" customHeight="1">
+    <row r="683" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D683" s="3"/>
     </row>
-    <row r="684" spans="4:4" ht="15.75" customHeight="1">
+    <row r="684" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D684" s="3"/>
     </row>
-    <row r="685" spans="4:4" ht="15.75" customHeight="1">
+    <row r="685" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D685" s="3"/>
     </row>
-    <row r="686" spans="4:4" ht="15.75" customHeight="1">
+    <row r="686" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D686" s="3"/>
     </row>
-    <row r="687" spans="4:4" ht="15.75" customHeight="1">
+    <row r="687" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D687" s="3"/>
     </row>
-    <row r="688" spans="4:4" ht="15.75" customHeight="1">
+    <row r="688" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D688" s="3"/>
     </row>
-    <row r="689" spans="4:4" ht="15.75" customHeight="1">
+    <row r="689" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D689" s="3"/>
     </row>
-    <row r="690" spans="4:4" ht="15.75" customHeight="1">
+    <row r="690" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D690" s="3"/>
     </row>
-    <row r="691" spans="4:4" ht="15.75" customHeight="1">
+    <row r="691" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D691" s="3"/>
     </row>
-    <row r="692" spans="4:4" ht="15.75" customHeight="1">
+    <row r="692" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D692" s="3"/>
     </row>
-    <row r="693" spans="4:4" ht="15.75" customHeight="1">
+    <row r="693" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D693" s="3"/>
     </row>
-    <row r="694" spans="4:4" ht="15.75" customHeight="1">
+    <row r="694" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D694" s="3"/>
     </row>
-    <row r="695" spans="4:4" ht="15.75" customHeight="1">
+    <row r="695" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D695" s="3"/>
     </row>
-    <row r="696" spans="4:4" ht="15.75" customHeight="1">
+    <row r="696" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D696" s="3"/>
     </row>
-    <row r="697" spans="4:4" ht="15.75" customHeight="1">
+    <row r="697" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D697" s="3"/>
     </row>
-    <row r="698" spans="4:4" ht="15.75" customHeight="1">
+    <row r="698" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D698" s="3"/>
     </row>
-    <row r="699" spans="4:4" ht="15.75" customHeight="1">
+    <row r="699" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D699" s="3"/>
     </row>
-    <row r="700" spans="4:4" ht="15.75" customHeight="1">
+    <row r="700" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D700" s="3"/>
     </row>
-    <row r="701" spans="4:4" ht="15.75" customHeight="1">
+    <row r="701" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D701" s="3"/>
     </row>
-    <row r="702" spans="4:4" ht="15.75" customHeight="1">
+    <row r="702" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D702" s="3"/>
     </row>
-    <row r="703" spans="4:4" ht="15.75" customHeight="1">
+    <row r="703" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D703" s="3"/>
     </row>
-    <row r="704" spans="4:4" ht="15.75" customHeight="1">
+    <row r="704" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D704" s="3"/>
     </row>
-    <row r="705" spans="4:4" ht="15.75" customHeight="1">
+    <row r="705" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D705" s="3"/>
     </row>
-    <row r="706" spans="4:4" ht="15.75" customHeight="1">
+    <row r="706" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D706" s="3"/>
     </row>
-    <row r="707" spans="4:4" ht="15.75" customHeight="1">
+    <row r="707" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D707" s="3"/>
     </row>
-    <row r="708" spans="4:4" ht="15.75" customHeight="1">
+    <row r="708" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D708" s="3"/>
     </row>
-    <row r="709" spans="4:4" ht="15.75" customHeight="1">
+    <row r="709" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D709" s="3"/>
     </row>
-    <row r="710" spans="4:4" ht="15.75" customHeight="1">
+    <row r="710" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D710" s="3"/>
     </row>
-    <row r="711" spans="4:4" ht="15.75" customHeight="1">
+    <row r="711" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D711" s="3"/>
     </row>
-    <row r="712" spans="4:4" ht="15.75" customHeight="1">
+    <row r="712" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D712" s="3"/>
     </row>
-    <row r="713" spans="4:4" ht="15.75" customHeight="1">
+    <row r="713" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D713" s="3"/>
     </row>
-    <row r="714" spans="4:4" ht="15.75" customHeight="1">
+    <row r="714" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D714" s="3"/>
     </row>
-    <row r="715" spans="4:4" ht="15.75" customHeight="1">
+    <row r="715" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D715" s="3"/>
     </row>
-    <row r="716" spans="4:4" ht="15.75" customHeight="1">
+    <row r="716" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D716" s="3"/>
     </row>
-    <row r="717" spans="4:4" ht="15.75" customHeight="1">
+    <row r="717" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D717" s="3"/>
     </row>
-    <row r="718" spans="4:4" ht="15.75" customHeight="1">
+    <row r="718" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D718" s="3"/>
     </row>
-    <row r="719" spans="4:4" ht="15.75" customHeight="1">
+    <row r="719" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D719" s="3"/>
     </row>
-    <row r="720" spans="4:4" ht="15.75" customHeight="1">
+    <row r="720" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D720" s="3"/>
     </row>
-    <row r="721" spans="4:4" ht="15.75" customHeight="1">
+    <row r="721" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D721" s="3"/>
     </row>
-    <row r="722" spans="4:4" ht="15.75" customHeight="1">
+    <row r="722" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D722" s="3"/>
     </row>
-    <row r="723" spans="4:4" ht="15.75" customHeight="1">
+    <row r="723" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D723" s="3"/>
     </row>
-    <row r="724" spans="4:4" ht="15.75" customHeight="1">
+    <row r="724" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D724" s="3"/>
     </row>
-    <row r="725" spans="4:4" ht="15.75" customHeight="1">
+    <row r="725" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D725" s="3"/>
     </row>
-    <row r="726" spans="4:4" ht="15.75" customHeight="1">
+    <row r="726" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D726" s="3"/>
     </row>
-    <row r="727" spans="4:4" ht="15.75" customHeight="1">
+    <row r="727" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D727" s="3"/>
     </row>
-    <row r="728" spans="4:4" ht="15.75" customHeight="1">
+    <row r="728" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D728" s="3"/>
     </row>
-    <row r="729" spans="4:4" ht="15.75" customHeight="1">
+    <row r="729" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D729" s="3"/>
     </row>
-    <row r="730" spans="4:4" ht="15.75" customHeight="1">
+    <row r="730" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D730" s="3"/>
     </row>
-    <row r="731" spans="4:4" ht="15.75" customHeight="1">
+    <row r="731" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D731" s="3"/>
     </row>
-    <row r="732" spans="4:4" ht="15.75" customHeight="1">
+    <row r="732" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D732" s="3"/>
     </row>
-    <row r="733" spans="4:4" ht="15.75" customHeight="1">
+    <row r="733" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D733" s="3"/>
     </row>
-    <row r="734" spans="4:4" ht="15.75" customHeight="1">
+    <row r="734" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D734" s="3"/>
     </row>
-    <row r="735" spans="4:4" ht="15.75" customHeight="1">
+    <row r="735" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D735" s="3"/>
     </row>
-    <row r="736" spans="4:4" ht="15.75" customHeight="1">
+    <row r="736" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D736" s="3"/>
     </row>
-    <row r="737" spans="4:4" ht="15.75" customHeight="1">
+    <row r="737" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D737" s="3"/>
     </row>
-    <row r="738" spans="4:4" ht="15.75" customHeight="1">
+    <row r="738" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D738" s="3"/>
     </row>
-    <row r="739" spans="4:4" ht="15.75" customHeight="1">
+    <row r="739" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D739" s="3"/>
     </row>
-    <row r="740" spans="4:4" ht="15.75" customHeight="1">
+    <row r="740" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D740" s="3"/>
     </row>
-    <row r="741" spans="4:4" ht="15.75" customHeight="1">
+    <row r="741" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D741" s="3"/>
     </row>
-    <row r="742" spans="4:4" ht="15.75" customHeight="1">
+    <row r="742" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D742" s="3"/>
     </row>
-    <row r="743" spans="4:4" ht="15.75" customHeight="1">
+    <row r="743" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D743" s="3"/>
     </row>
-    <row r="744" spans="4:4" ht="15.75" customHeight="1">
+    <row r="744" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D744" s="3"/>
     </row>
-    <row r="745" spans="4:4" ht="15.75" customHeight="1">
+    <row r="745" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D745" s="3"/>
     </row>
-    <row r="746" spans="4:4" ht="15.75" customHeight="1">
+    <row r="746" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D746" s="3"/>
     </row>
-    <row r="747" spans="4:4" ht="15.75" customHeight="1">
+    <row r="747" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D747" s="3"/>
     </row>
-    <row r="748" spans="4:4" ht="15.75" customHeight="1">
+    <row r="748" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D748" s="3"/>
     </row>
-    <row r="749" spans="4:4" ht="15.75" customHeight="1">
+    <row r="749" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D749" s="3"/>
     </row>
-    <row r="750" spans="4:4" ht="15.75" customHeight="1">
+    <row r="750" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D750" s="3"/>
     </row>
-    <row r="751" spans="4:4" ht="15.75" customHeight="1">
+    <row r="751" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D751" s="3"/>
     </row>
-    <row r="752" spans="4:4" ht="15.75" customHeight="1">
+    <row r="752" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D752" s="3"/>
     </row>
-    <row r="753" spans="4:4" ht="15.75" customHeight="1">
+    <row r="753" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D753" s="3"/>
     </row>
-    <row r="754" spans="4:4" ht="15.75" customHeight="1">
+    <row r="754" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D754" s="3"/>
     </row>
-    <row r="755" spans="4:4" ht="15.75" customHeight="1">
+    <row r="755" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D755" s="3"/>
     </row>
-    <row r="756" spans="4:4" ht="15.75" customHeight="1">
+    <row r="756" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D756" s="3"/>
     </row>
-    <row r="757" spans="4:4" ht="15.75" customHeight="1">
+    <row r="757" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D757" s="3"/>
     </row>
-    <row r="758" spans="4:4" ht="15.75" customHeight="1">
+    <row r="758" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D758" s="3"/>
     </row>
-    <row r="759" spans="4:4" ht="15.75" customHeight="1">
+    <row r="759" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D759" s="3"/>
     </row>
-    <row r="760" spans="4:4" ht="15.75" customHeight="1">
+    <row r="760" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D760" s="3"/>
     </row>
-    <row r="761" spans="4:4" ht="15.75" customHeight="1">
+    <row r="761" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D761" s="3"/>
     </row>
-    <row r="762" spans="4:4" ht="15.75" customHeight="1">
+    <row r="762" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D762" s="3"/>
     </row>
-    <row r="763" spans="4:4" ht="15.75" customHeight="1">
+    <row r="763" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D763" s="3"/>
     </row>
-    <row r="764" spans="4:4" ht="15.75" customHeight="1">
+    <row r="764" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D764" s="3"/>
     </row>
-    <row r="765" spans="4:4" ht="15.75" customHeight="1">
+    <row r="765" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D765" s="3"/>
     </row>
-    <row r="766" spans="4:4" ht="15.75" customHeight="1">
+    <row r="766" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D766" s="3"/>
     </row>
-    <row r="767" spans="4:4" ht="15.75" customHeight="1">
+    <row r="767" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D767" s="3"/>
     </row>
-    <row r="768" spans="4:4" ht="15.75" customHeight="1">
+    <row r="768" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D768" s="3"/>
     </row>
-    <row r="769" spans="4:4" ht="15.75" customHeight="1">
+    <row r="769" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D769" s="3"/>
     </row>
-    <row r="770" spans="4:4" ht="15.75" customHeight="1">
+    <row r="770" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D770" s="3"/>
     </row>
-    <row r="771" spans="4:4" ht="15.75" customHeight="1">
+    <row r="771" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D771" s="3"/>
     </row>
-    <row r="772" spans="4:4" ht="15.75" customHeight="1">
+    <row r="772" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D772" s="3"/>
     </row>
-    <row r="773" spans="4:4" ht="15.75" customHeight="1">
+    <row r="773" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D773" s="3"/>
     </row>
-    <row r="774" spans="4:4" ht="15.75" customHeight="1">
+    <row r="774" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D774" s="3"/>
     </row>
-    <row r="775" spans="4:4" ht="15.75" customHeight="1">
+    <row r="775" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D775" s="3"/>
     </row>
-    <row r="776" spans="4:4" ht="15.75" customHeight="1">
+    <row r="776" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D776" s="3"/>
     </row>
-    <row r="777" spans="4:4" ht="15.75" customHeight="1">
+    <row r="777" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D777" s="3"/>
     </row>
-    <row r="778" spans="4:4" ht="15.75" customHeight="1">
+    <row r="778" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D778" s="3"/>
     </row>
-    <row r="779" spans="4:4" ht="15.75" customHeight="1">
+    <row r="779" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D779" s="3"/>
     </row>
-    <row r="780" spans="4:4" ht="15.75" customHeight="1">
+    <row r="780" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D780" s="3"/>
     </row>
-    <row r="781" spans="4:4" ht="15.75" customHeight="1">
+    <row r="781" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D781" s="3"/>
     </row>
-    <row r="782" spans="4:4" ht="15.75" customHeight="1">
+    <row r="782" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D782" s="3"/>
     </row>
-    <row r="783" spans="4:4" ht="15.75" customHeight="1">
+    <row r="783" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D783" s="3"/>
     </row>
-    <row r="784" spans="4:4" ht="15.75" customHeight="1">
+    <row r="784" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D784" s="3"/>
     </row>
-    <row r="785" spans="4:4" ht="15.75" customHeight="1">
+    <row r="785" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D785" s="3"/>
     </row>
-    <row r="786" spans="4:4" ht="15.75" customHeight="1">
+    <row r="786" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D786" s="3"/>
     </row>
-    <row r="787" spans="4:4" ht="15.75" customHeight="1">
+    <row r="787" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D787" s="3"/>
     </row>
-    <row r="788" spans="4:4" ht="15.75" customHeight="1">
+    <row r="788" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D788" s="3"/>
     </row>
-    <row r="789" spans="4:4" ht="15.75" customHeight="1">
+    <row r="789" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D789" s="3"/>
     </row>
-    <row r="790" spans="4:4" ht="15.75" customHeight="1">
+    <row r="790" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D790" s="3"/>
     </row>
-    <row r="791" spans="4:4" ht="15.75" customHeight="1">
+    <row r="791" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D791" s="3"/>
     </row>
-    <row r="792" spans="4:4" ht="15.75" customHeight="1">
+    <row r="792" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D792" s="3"/>
     </row>
-    <row r="793" spans="4:4" ht="15.75" customHeight="1">
+    <row r="793" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D793" s="3"/>
     </row>
-    <row r="794" spans="4:4" ht="15.75" customHeight="1">
+    <row r="794" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D794" s="3"/>
     </row>
-    <row r="795" spans="4:4" ht="15.75" customHeight="1">
+    <row r="795" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D795" s="3"/>
     </row>
-    <row r="796" spans="4:4" ht="15.75" customHeight="1">
+    <row r="796" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D796" s="3"/>
     </row>
-    <row r="797" spans="4:4" ht="15.75" customHeight="1">
+    <row r="797" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D797" s="3"/>
     </row>
-    <row r="798" spans="4:4" ht="15.75" customHeight="1">
+    <row r="798" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D798" s="3"/>
     </row>
-    <row r="799" spans="4:4" ht="15.75" customHeight="1">
+    <row r="799" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D799" s="3"/>
     </row>
-    <row r="800" spans="4:4" ht="15.75" customHeight="1">
+    <row r="800" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D800" s="3"/>
     </row>
-    <row r="801" spans="4:4" ht="15.75" customHeight="1">
+    <row r="801" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D801" s="3"/>
     </row>
-    <row r="802" spans="4:4" ht="15.75" customHeight="1">
+    <row r="802" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D802" s="3"/>
     </row>
-    <row r="803" spans="4:4" ht="15.75" customHeight="1">
+    <row r="803" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D803" s="3"/>
     </row>
-    <row r="804" spans="4:4" ht="15.75" customHeight="1">
+    <row r="804" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D804" s="3"/>
     </row>
-    <row r="805" spans="4:4" ht="15.75" customHeight="1">
+    <row r="805" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D805" s="3"/>
     </row>
-    <row r="806" spans="4:4" ht="15.75" customHeight="1">
+    <row r="806" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D806" s="3"/>
     </row>
-    <row r="807" spans="4:4" ht="15.75" customHeight="1">
+    <row r="807" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D807" s="3"/>
     </row>
-    <row r="808" spans="4:4" ht="15.75" customHeight="1">
+    <row r="808" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D808" s="3"/>
     </row>
-    <row r="809" spans="4:4" ht="15.75" customHeight="1">
+    <row r="809" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D809" s="3"/>
     </row>
-    <row r="810" spans="4:4" ht="15.75" customHeight="1">
+    <row r="810" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D810" s="3"/>
     </row>
-    <row r="811" spans="4:4" ht="15.75" customHeight="1">
+    <row r="811" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D811" s="3"/>
     </row>
-    <row r="812" spans="4:4" ht="15.75" customHeight="1">
+    <row r="812" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D812" s="3"/>
     </row>
-    <row r="813" spans="4:4" ht="15.75" customHeight="1">
+    <row r="813" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D813" s="3"/>
     </row>
-    <row r="814" spans="4:4" ht="15.75" customHeight="1">
+    <row r="814" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D814" s="3"/>
     </row>
-    <row r="815" spans="4:4" ht="15.75" customHeight="1">
+    <row r="815" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D815" s="3"/>
     </row>
-    <row r="816" spans="4:4" ht="15.75" customHeight="1">
+    <row r="816" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D816" s="3"/>
     </row>
-    <row r="817" spans="4:4" ht="15.75" customHeight="1">
+    <row r="817" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D817" s="3"/>
     </row>
-    <row r="818" spans="4:4" ht="15.75" customHeight="1">
+    <row r="818" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D818" s="3"/>
     </row>
-    <row r="819" spans="4:4" ht="15.75" customHeight="1">
+    <row r="819" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D819" s="3"/>
     </row>
-    <row r="820" spans="4:4" ht="15.75" customHeight="1">
+    <row r="820" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D820" s="3"/>
     </row>
-    <row r="821" spans="4:4" ht="15.75" customHeight="1">
+    <row r="821" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D821" s="3"/>
     </row>
-    <row r="822" spans="4:4" ht="15.75" customHeight="1">
+    <row r="822" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D822" s="3"/>
     </row>
-    <row r="823" spans="4:4" ht="15.75" customHeight="1">
+    <row r="823" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D823" s="3"/>
     </row>
-    <row r="824" spans="4:4" ht="15.75" customHeight="1">
+    <row r="824" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D824" s="3"/>
     </row>
-    <row r="825" spans="4:4" ht="15.75" customHeight="1">
+    <row r="825" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D825" s="3"/>
     </row>
-    <row r="826" spans="4:4" ht="15.75" customHeight="1">
+    <row r="826" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D826" s="3"/>
     </row>
-    <row r="827" spans="4:4" ht="15.75" customHeight="1">
+    <row r="827" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D827" s="3"/>
     </row>
-    <row r="828" spans="4:4" ht="15.75" customHeight="1">
+    <row r="828" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D828" s="3"/>
     </row>
-    <row r="829" spans="4:4" ht="15.75" customHeight="1">
+    <row r="829" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D829" s="3"/>
     </row>
-    <row r="830" spans="4:4" ht="15.75" customHeight="1">
+    <row r="830" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D830" s="3"/>
     </row>
-    <row r="831" spans="4:4" ht="15.75" customHeight="1">
+    <row r="831" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D831" s="3"/>
     </row>
-    <row r="832" spans="4:4" ht="15.75" customHeight="1">
+    <row r="832" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D832" s="3"/>
     </row>
-    <row r="833" spans="4:4" ht="15.75" customHeight="1">
+    <row r="833" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D833" s="3"/>
     </row>
-    <row r="834" spans="4:4" ht="15.75" customHeight="1">
+    <row r="834" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D834" s="3"/>
     </row>
-    <row r="835" spans="4:4" ht="15.75" customHeight="1">
+    <row r="835" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D835" s="3"/>
     </row>
-    <row r="836" spans="4:4" ht="15.75" customHeight="1">
+    <row r="836" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D836" s="3"/>
     </row>
-    <row r="837" spans="4:4" ht="15.75" customHeight="1">
+    <row r="837" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D837" s="3"/>
     </row>
-    <row r="838" spans="4:4" ht="15.75" customHeight="1">
+    <row r="838" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D838" s="3"/>
     </row>
-    <row r="839" spans="4:4" ht="15.75" customHeight="1">
+    <row r="839" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D839" s="3"/>
     </row>
-    <row r="840" spans="4:4" ht="15.75" customHeight="1">
+    <row r="840" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D840" s="3"/>
     </row>
-    <row r="841" spans="4:4" ht="15.75" customHeight="1">
+    <row r="841" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D841" s="3"/>
     </row>
-    <row r="842" spans="4:4" ht="15.75" customHeight="1">
+    <row r="842" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D842" s="3"/>
     </row>
-    <row r="843" spans="4:4" ht="15.75" customHeight="1">
+    <row r="843" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D843" s="3"/>
     </row>
-    <row r="844" spans="4:4" ht="15.75" customHeight="1">
+    <row r="844" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D844" s="3"/>
     </row>
-    <row r="845" spans="4:4" ht="15.75" customHeight="1">
+    <row r="845" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D845" s="3"/>
     </row>
-    <row r="846" spans="4:4" ht="15.75" customHeight="1">
+    <row r="846" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D846" s="3"/>
     </row>
-    <row r="847" spans="4:4" ht="15.75" customHeight="1">
+    <row r="847" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D847" s="3"/>
     </row>
-    <row r="848" spans="4:4" ht="15.75" customHeight="1">
+    <row r="848" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D848" s="3"/>
     </row>
-    <row r="849" spans="4:4" ht="15.75" customHeight="1">
+    <row r="849" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D849" s="3"/>
     </row>
-    <row r="850" spans="4:4" ht="15.75" customHeight="1">
+    <row r="850" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D850" s="3"/>
     </row>
-    <row r="851" spans="4:4" ht="15.75" customHeight="1">
+    <row r="851" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D851" s="3"/>
     </row>
-    <row r="852" spans="4:4" ht="15.75" customHeight="1">
+    <row r="852" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D852" s="3"/>
     </row>
-    <row r="853" spans="4:4" ht="15.75" customHeight="1">
+    <row r="853" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D853" s="3"/>
     </row>
-    <row r="854" spans="4:4" ht="15.75" customHeight="1">
+    <row r="854" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D854" s="3"/>
     </row>
-    <row r="855" spans="4:4" ht="15.75" customHeight="1">
+    <row r="855" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D855" s="3"/>
     </row>
-    <row r="856" spans="4:4" ht="15.75" customHeight="1">
+    <row r="856" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D856" s="3"/>
     </row>
-    <row r="857" spans="4:4" ht="15.75" customHeight="1">
+    <row r="857" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D857" s="3"/>
     </row>
-    <row r="858" spans="4:4" ht="15.75" customHeight="1">
+    <row r="858" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D858" s="3"/>
     </row>
-    <row r="859" spans="4:4" ht="15.75" customHeight="1">
+    <row r="859" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D859" s="3"/>
     </row>
-    <row r="860" spans="4:4" ht="15.75" customHeight="1">
+    <row r="860" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D860" s="3"/>
     </row>
-    <row r="861" spans="4:4" ht="15.75" customHeight="1">
+    <row r="861" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D861" s="3"/>
     </row>
-    <row r="862" spans="4:4" ht="15.75" customHeight="1">
+    <row r="862" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D862" s="3"/>
     </row>
-    <row r="863" spans="4:4" ht="15.75" customHeight="1">
+    <row r="863" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D863" s="3"/>
     </row>
-    <row r="864" spans="4:4" ht="15.75" customHeight="1">
+    <row r="864" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D864" s="3"/>
     </row>
-    <row r="865" spans="4:4" ht="15.75" customHeight="1">
+    <row r="865" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D865" s="3"/>
     </row>
-    <row r="866" spans="4:4" ht="15.75" customHeight="1">
+    <row r="866" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D866" s="3"/>
     </row>
-    <row r="867" spans="4:4" ht="15.75" customHeight="1">
+    <row r="867" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D867" s="3"/>
     </row>
-    <row r="868" spans="4:4" ht="15.75" customHeight="1">
+    <row r="868" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D868" s="3"/>
     </row>
-    <row r="869" spans="4:4" ht="15.75" customHeight="1">
+    <row r="869" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D869" s="3"/>
     </row>
-    <row r="870" spans="4:4" ht="15.75" customHeight="1">
+    <row r="870" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D870" s="3"/>
     </row>
-    <row r="871" spans="4:4" ht="15.75" customHeight="1">
+    <row r="871" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D871" s="3"/>
     </row>
-    <row r="872" spans="4:4" ht="15.75" customHeight="1">
+    <row r="872" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D872" s="3"/>
     </row>
-    <row r="873" spans="4:4" ht="15.75" customHeight="1">
+    <row r="873" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D873" s="3"/>
     </row>
-    <row r="874" spans="4:4" ht="15.75" customHeight="1">
+    <row r="874" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D874" s="3"/>
     </row>
-    <row r="875" spans="4:4" ht="15.75" customHeight="1">
+    <row r="875" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D875" s="3"/>
     </row>
-    <row r="876" spans="4:4" ht="15.75" customHeight="1">
+    <row r="876" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D876" s="3"/>
     </row>
-    <row r="877" spans="4:4" ht="15.75" customHeight="1">
+    <row r="877" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D877" s="3"/>
     </row>
-    <row r="878" spans="4:4" ht="15.75" customHeight="1">
+    <row r="878" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D878" s="3"/>
     </row>
-    <row r="879" spans="4:4" ht="15.75" customHeight="1">
+    <row r="879" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D879" s="3"/>
     </row>
-    <row r="880" spans="4:4" ht="15.75" customHeight="1">
+    <row r="880" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D880" s="3"/>
     </row>
-    <row r="881" spans="4:4" ht="15.75" customHeight="1">
+    <row r="881" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D881" s="3"/>
     </row>
-    <row r="882" spans="4:4" ht="15.75" customHeight="1">
+    <row r="882" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D882" s="3"/>
     </row>
-    <row r="883" spans="4:4" ht="15.75" customHeight="1">
+    <row r="883" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D883" s="3"/>
     </row>
-    <row r="884" spans="4:4" ht="15.75" customHeight="1">
+    <row r="884" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D884" s="3"/>
     </row>
-    <row r="885" spans="4:4" ht="15.75" customHeight="1">
+    <row r="885" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D885" s="3"/>
     </row>
-    <row r="886" spans="4:4" ht="15.75" customHeight="1">
+    <row r="886" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D886" s="3"/>
     </row>
-    <row r="887" spans="4:4" ht="15.75" customHeight="1">
+    <row r="887" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D887" s="3"/>
     </row>
-    <row r="888" spans="4:4" ht="15.75" customHeight="1">
+    <row r="888" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D888" s="3"/>
     </row>
-    <row r="889" spans="4:4" ht="15.75" customHeight="1">
+    <row r="889" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D889" s="3"/>
     </row>
-    <row r="890" spans="4:4" ht="15.75" customHeight="1">
+    <row r="890" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D890" s="3"/>
     </row>
-    <row r="891" spans="4:4" ht="15.75" customHeight="1">
+    <row r="891" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D891" s="3"/>
     </row>
-    <row r="892" spans="4:4" ht="15.75" customHeight="1">
+    <row r="892" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D892" s="3"/>
     </row>
-    <row r="893" spans="4:4" ht="15.75" customHeight="1">
+    <row r="893" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D893" s="3"/>
     </row>
-    <row r="894" spans="4:4" ht="15.75" customHeight="1">
+    <row r="894" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D894" s="3"/>
     </row>
-    <row r="895" spans="4:4" ht="15.75" customHeight="1">
+    <row r="895" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D895" s="3"/>
     </row>
-    <row r="896" spans="4:4" ht="15.75" customHeight="1">
+    <row r="896" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D896" s="3"/>
     </row>
-    <row r="897" spans="4:4" ht="15.75" customHeight="1">
+    <row r="897" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D897" s="3"/>
     </row>
-    <row r="898" spans="4:4" ht="15.75" customHeight="1">
+    <row r="898" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D898" s="3"/>
     </row>
-    <row r="899" spans="4:4" ht="15.75" customHeight="1">
+    <row r="899" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D899" s="3"/>
     </row>
-    <row r="900" spans="4:4" ht="15.75" customHeight="1">
+    <row r="900" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D900" s="3"/>
     </row>
-    <row r="901" spans="4:4" ht="15.75" customHeight="1">
+    <row r="901" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D901" s="3"/>
     </row>
-    <row r="902" spans="4:4" ht="15.75" customHeight="1">
+    <row r="902" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D902" s="3"/>
     </row>
-    <row r="903" spans="4:4" ht="15.75" customHeight="1">
+    <row r="903" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D903" s="3"/>
     </row>
-    <row r="904" spans="4:4" ht="15.75" customHeight="1">
+    <row r="904" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D904" s="3"/>
     </row>
-    <row r="905" spans="4:4" ht="15.75" customHeight="1">
+    <row r="905" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D905" s="3"/>
     </row>
-    <row r="906" spans="4:4" ht="15.75" customHeight="1">
+    <row r="906" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D906" s="3"/>
     </row>
-    <row r="907" spans="4:4" ht="15.75" customHeight="1">
+    <row r="907" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D907" s="3"/>
     </row>
-    <row r="908" spans="4:4" ht="15.75" customHeight="1">
+    <row r="908" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D908" s="3"/>
     </row>
-    <row r="909" spans="4:4" ht="15.75" customHeight="1">
+    <row r="909" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D909" s="3"/>
     </row>
-    <row r="910" spans="4:4" ht="15.75" customHeight="1">
+    <row r="910" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D910" s="3"/>
     </row>
-    <row r="911" spans="4:4" ht="15.75" customHeight="1">
+    <row r="911" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D911" s="3"/>
     </row>
-    <row r="912" spans="4:4" ht="15.75" customHeight="1">
+    <row r="912" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D912" s="3"/>
     </row>
-    <row r="913" spans="4:4" ht="15.75" customHeight="1">
+    <row r="913" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D913" s="3"/>
     </row>
-    <row r="914" spans="4:4" ht="15.75" customHeight="1">
+    <row r="914" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D914" s="3"/>
     </row>
-    <row r="915" spans="4:4" ht="15.75" customHeight="1">
+    <row r="915" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D915" s="3"/>
     </row>
-    <row r="916" spans="4:4" ht="15.75" customHeight="1">
+    <row r="916" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D916" s="3"/>
     </row>
-    <row r="917" spans="4:4" ht="15.75" customHeight="1">
+    <row r="917" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D917" s="3"/>
     </row>
-    <row r="918" spans="4:4" ht="15.75" customHeight="1">
+    <row r="918" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D918" s="3"/>
     </row>
-    <row r="919" spans="4:4" ht="15.75" customHeight="1">
+    <row r="919" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D919" s="3"/>
     </row>
-    <row r="920" spans="4:4" ht="15.75" customHeight="1">
+    <row r="920" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D920" s="3"/>
     </row>
-    <row r="921" spans="4:4" ht="15.75" customHeight="1">
+    <row r="921" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D921" s="3"/>
     </row>
-    <row r="922" spans="4:4" ht="15.75" customHeight="1">
+    <row r="922" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D922" s="3"/>
     </row>
-    <row r="923" spans="4:4" ht="15.75" customHeight="1">
+    <row r="923" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D923" s="3"/>
     </row>
-    <row r="924" spans="4:4" ht="15.75" customHeight="1">
+    <row r="924" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D924" s="3"/>
     </row>
-    <row r="925" spans="4:4" ht="15.75" customHeight="1">
+    <row r="925" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D925" s="3"/>
     </row>
-    <row r="926" spans="4:4" ht="15.75" customHeight="1">
+    <row r="926" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D926" s="3"/>
     </row>
-    <row r="927" spans="4:4" ht="15.75" customHeight="1">
+    <row r="927" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D927" s="3"/>
     </row>
-    <row r="928" spans="4:4" ht="15.75" customHeight="1">
+    <row r="928" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D928" s="3"/>
     </row>
-    <row r="929" spans="4:4" ht="15.75" customHeight="1">
+    <row r="929" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D929" s="3"/>
     </row>
-    <row r="930" spans="4:4" ht="15.75" customHeight="1">
+    <row r="930" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D930" s="3"/>
     </row>
-    <row r="931" spans="4:4" ht="15.75" customHeight="1">
+    <row r="931" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D931" s="3"/>
     </row>
-    <row r="932" spans="4:4" ht="15.75" customHeight="1">
+    <row r="932" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D932" s="3"/>
     </row>
-    <row r="933" spans="4:4" ht="15.75" customHeight="1">
+    <row r="933" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D933" s="3"/>
     </row>
-    <row r="934" spans="4:4" ht="15.75" customHeight="1">
+    <row r="934" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D934" s="3"/>
     </row>
-    <row r="935" spans="4:4" ht="15.75" customHeight="1">
+    <row r="935" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D935" s="3"/>
     </row>
-    <row r="936" spans="4:4" ht="15.75" customHeight="1">
+    <row r="936" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D936" s="3"/>
     </row>
-    <row r="937" spans="4:4" ht="15.75" customHeight="1">
+    <row r="937" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D937" s="3"/>
     </row>
-    <row r="938" spans="4:4" ht="15.75" customHeight="1">
+    <row r="938" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D938" s="3"/>
     </row>
-    <row r="939" spans="4:4" ht="15.75" customHeight="1">
+    <row r="939" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D939" s="3"/>
     </row>
-    <row r="940" spans="4:4" ht="15.75" customHeight="1">
+    <row r="940" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D940" s="3"/>
     </row>
-    <row r="941" spans="4:4" ht="15.75" customHeight="1">
+    <row r="941" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D941" s="3"/>
     </row>
-    <row r="942" spans="4:4" ht="15.75" customHeight="1">
+    <row r="942" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D942" s="3"/>
     </row>
-    <row r="943" spans="4:4" ht="15.75" customHeight="1">
+    <row r="943" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D943" s="3"/>
     </row>
-    <row r="944" spans="4:4" ht="15.75" customHeight="1">
+    <row r="944" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D944" s="3"/>
     </row>
-    <row r="945" spans="4:4" ht="15.75" customHeight="1">
+    <row r="945" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D945" s="3"/>
     </row>
-    <row r="946" spans="4:4" ht="15.75" customHeight="1">
+    <row r="946" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D946" s="3"/>
     </row>
-    <row r="947" spans="4:4" ht="15.75" customHeight="1">
+    <row r="947" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D947" s="3"/>
     </row>
-    <row r="948" spans="4:4" ht="15.75" customHeight="1">
+    <row r="948" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D948" s="3"/>
     </row>
-    <row r="949" spans="4:4" ht="15.75" customHeight="1">
+    <row r="949" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D949" s="3"/>
     </row>
-    <row r="950" spans="4:4" ht="15.75" customHeight="1">
+    <row r="950" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D950" s="3"/>
     </row>
-    <row r="951" spans="4:4" ht="15.75" customHeight="1">
+    <row r="951" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D951" s="3"/>
     </row>
-    <row r="952" spans="4:4" ht="15.75" customHeight="1">
+    <row r="952" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D952" s="3"/>
     </row>
-    <row r="953" spans="4:4" ht="15.75" customHeight="1">
+    <row r="953" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D953" s="3"/>
     </row>
-    <row r="954" spans="4:4" ht="15.75" customHeight="1">
+    <row r="954" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D954" s="3"/>
     </row>
-    <row r="955" spans="4:4" ht="15.75" customHeight="1">
+    <row r="955" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D955" s="3"/>
     </row>
-    <row r="956" spans="4:4" ht="15.75" customHeight="1">
+    <row r="956" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D956" s="3"/>
     </row>
-    <row r="957" spans="4:4" ht="15.75" customHeight="1">
+    <row r="957" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D957" s="3"/>
     </row>
-    <row r="958" spans="4:4" ht="15.75" customHeight="1">
+    <row r="958" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D958" s="3"/>
     </row>
-    <row r="959" spans="4:4" ht="15.75" customHeight="1">
+    <row r="959" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D959" s="3"/>
     </row>
-    <row r="960" spans="4:4" ht="15.75" customHeight="1">
+    <row r="960" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D960" s="3"/>
     </row>
-    <row r="961" spans="4:4" ht="15.75" customHeight="1">
+    <row r="961" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D961" s="3"/>
     </row>
-    <row r="962" spans="4:4" ht="15.75" customHeight="1">
+    <row r="962" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D962" s="3"/>
     </row>
-    <row r="963" spans="4:4" ht="15.75" customHeight="1">
+    <row r="963" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D963" s="3"/>
     </row>
-    <row r="964" spans="4:4" ht="15.75" customHeight="1">
+    <row r="964" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D964" s="3"/>
     </row>
-    <row r="965" spans="4:4" ht="15.75" customHeight="1">
+    <row r="965" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D965" s="3"/>
     </row>
-    <row r="966" spans="4:4" ht="15.75" customHeight="1">
+    <row r="966" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D966" s="3"/>
     </row>
-    <row r="967" spans="4:4" ht="15.75" customHeight="1">
+    <row r="967" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D967" s="3"/>
     </row>
-    <row r="968" spans="4:4" ht="15.75" customHeight="1">
+    <row r="968" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D968" s="3"/>
     </row>
-    <row r="969" spans="4:4" ht="15.75" customHeight="1">
+    <row r="969" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D969" s="3"/>
     </row>
-    <row r="970" spans="4:4" ht="15.75" customHeight="1">
+    <row r="970" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D970" s="3"/>
     </row>
-    <row r="971" spans="4:4" ht="15.75" customHeight="1">
+    <row r="971" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D971" s="3"/>
     </row>
-    <row r="972" spans="4:4" ht="15.75" customHeight="1">
+    <row r="972" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D972" s="3"/>
     </row>
-    <row r="973" spans="4:4" ht="15.75" customHeight="1">
+    <row r="973" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D973" s="3"/>
     </row>
-    <row r="974" spans="4:4" ht="15.75" customHeight="1">
+    <row r="974" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D974" s="3"/>
     </row>
-    <row r="975" spans="4:4" ht="15.75" customHeight="1">
+    <row r="975" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D975" s="3"/>
     </row>
-    <row r="976" spans="4:4" ht="15.75" customHeight="1">
+    <row r="976" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D976" s="3"/>
     </row>
-    <row r="977" spans="4:4" ht="15.75" customHeight="1">
+    <row r="977" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D977" s="3"/>
     </row>
-    <row r="978" spans="4:4" ht="15.75" customHeight="1">
+    <row r="978" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D978" s="3"/>
     </row>
-    <row r="979" spans="4:4" ht="15.75" customHeight="1">
+    <row r="979" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D979" s="3"/>
     </row>
-    <row r="980" spans="4:4" ht="15.75" customHeight="1">
+    <row r="980" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D980" s="3"/>
     </row>
-    <row r="981" spans="4:4" ht="15.75" customHeight="1">
+    <row r="981" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D981" s="3"/>
     </row>
-    <row r="982" spans="4:4" ht="15.75" customHeight="1">
+    <row r="982" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D982" s="3"/>
     </row>
-    <row r="983" spans="4:4" ht="15.75" customHeight="1">
+    <row r="983" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D983" s="3"/>
     </row>
-    <row r="984" spans="4:4" ht="15.75" customHeight="1">
+    <row r="984" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D984" s="3"/>
     </row>
-    <row r="985" spans="4:4" ht="15.75" customHeight="1">
+    <row r="985" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D985" s="3"/>
     </row>
-    <row r="986" spans="4:4" ht="15.75" customHeight="1">
+    <row r="986" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D986" s="3"/>
     </row>
-    <row r="987" spans="4:4" ht="15.75" customHeight="1">
+    <row r="987" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D987" s="3"/>
     </row>
-    <row r="988" spans="4:4" ht="15.75" customHeight="1">
+    <row r="988" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D988" s="3"/>
     </row>
-    <row r="989" spans="4:4" ht="15.75" customHeight="1">
+    <row r="989" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D989" s="3"/>
     </row>
-    <row r="990" spans="4:4" ht="15.75" customHeight="1">
+    <row r="990" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D990" s="3"/>
     </row>
-    <row r="991" spans="4:4" ht="15.75" customHeight="1">
+    <row r="991" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D991" s="3"/>
     </row>
-    <row r="992" spans="4:4" ht="15.75" customHeight="1">
+    <row r="992" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D992" s="3"/>
     </row>
-    <row r="993" spans="4:4" ht="15.75" customHeight="1">
+    <row r="993" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D993" s="3"/>
     </row>
-    <row r="994" spans="4:4" ht="15.75" customHeight="1">
+    <row r="994" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D994" s="3"/>
     </row>
-    <row r="995" spans="4:4" ht="15.75" customHeight="1">
+    <row r="995" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D995" s="3"/>
     </row>
-    <row r="996" spans="4:4" ht="15.75" customHeight="1">
+    <row r="996" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D996" s="3"/>
     </row>
-    <row r="997" spans="4:4" ht="15.75" customHeight="1">
+    <row r="997" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D997" s="3"/>
     </row>
-    <row r="998" spans="4:4" ht="15.75" customHeight="1">
+    <row r="998" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D998" s="3"/>
     </row>
-    <row r="999" spans="4:4" ht="15.75" customHeight="1">
+    <row r="999" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D999" s="3"/>
     </row>
-    <row r="1000" spans="4:4" ht="15.75" customHeight="1">
+    <row r="1000" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D1000" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>